<commit_message>
updateXlsxWithCardsUrl update -> create new page with current date as name in the input xlsx file and write cards url with filters -> test ok
</commit_message>
<xml_diff>
--- a/excelPriceCards/cartes.xlsx
+++ b/excelPriceCards/cartes.xlsx
@@ -4,6 +4,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="27_01_2024" sheetId="2" r:id="rId2"/>
   </sheets>
 </workbook>
 </file>
@@ -415,6 +416,9 @@
       <c r="D1" t="str">
         <v>Langue</v>
       </c>
+      <c r="E1" t="str">
+        <v/>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -430,7 +434,7 @@
         <v>JP</v>
       </c>
       <c r="E2" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Eevee-Heroes/Umbreon-V-V3-s6a085</v>
+        <v/>
       </c>
     </row>
     <row r="3">
@@ -447,7 +451,7 @@
         <v>JP</v>
       </c>
       <c r="E3" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Eevee-Heroes/Glaceon-VMAX-V1</v>
+        <v/>
       </c>
     </row>
     <row r="4">
@@ -464,7 +468,7 @@
         <v>JP</v>
       </c>
       <c r="E4" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Eevee-Heroes/Sylveon-VMAX-V1-s6a041</v>
+        <v/>
       </c>
     </row>
     <row r="5">
@@ -481,7 +485,7 @@
         <v>JP</v>
       </c>
       <c r="E5" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Eevee-Heroes/Umbreon-VMAX-V1</v>
+        <v/>
       </c>
     </row>
     <row r="6">
@@ -498,7 +502,7 @@
         <v>JP</v>
       </c>
       <c r="E6" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Eevee-Heroes/Sylveon-V-V1</v>
+        <v/>
       </c>
     </row>
     <row r="7">
@@ -515,7 +519,7 @@
         <v>JP</v>
       </c>
       <c r="E7" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Eevee-Heroes/Glaceon-V-V1-s6a024</v>
+        <v/>
       </c>
     </row>
     <row r="8">
@@ -532,7 +536,7 @@
         <v>JP</v>
       </c>
       <c r="E8" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Eevee-Heroes/Vaporeon-V-V1</v>
+        <v/>
       </c>
     </row>
     <row r="9">
@@ -549,7 +553,7 @@
         <v>JP</v>
       </c>
       <c r="E9" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Eevee-Heroes/Leafeon-V-V1</v>
+        <v/>
       </c>
     </row>
     <row r="10">
@@ -566,7 +570,7 @@
         <v>JP</v>
       </c>
       <c r="E10" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Blue-Sky-Stream/Trevenant-V-V2</v>
+        <v/>
       </c>
     </row>
     <row r="11">
@@ -583,7 +587,7 @@
         <v>JP</v>
       </c>
       <c r="E11" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Blue-Sky-Stream/Gyarados-VMAX-V1</v>
+        <v/>
       </c>
     </row>
     <row r="12">
@@ -600,7 +604,7 @@
         <v>JP</v>
       </c>
       <c r="E12" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Blue-Sky-Stream/Rayquaza-VMAX-V1-s7R047</v>
+        <v/>
       </c>
     </row>
     <row r="13">
@@ -617,7 +621,7 @@
         <v>JP</v>
       </c>
       <c r="E13" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Blue-Sky-Stream/Gyarados-V-V1-s7R020</v>
+        <v/>
       </c>
     </row>
     <row r="14">
@@ -634,7 +638,7 @@
         <v>JP</v>
       </c>
       <c r="E14" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Blue-Sky-Stream/Rayquaza-V-V1</v>
+        <v/>
       </c>
     </row>
     <row r="15">
@@ -651,7 +655,7 @@
         <v>JP</v>
       </c>
       <c r="E15" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Blue-Sky-Stream/Volcarona-V-V1-s7R015</v>
+        <v/>
       </c>
     </row>
     <row r="16">
@@ -668,7 +672,7 @@
         <v>JP</v>
       </c>
       <c r="E16" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Blue-Sky-Stream/Trevenant-V-V1</v>
+        <v/>
       </c>
     </row>
     <row r="17">
@@ -685,7 +689,7 @@
         <v>JP</v>
       </c>
       <c r="E17" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Blue-Sky-Stream/Dragonite-V-V1</v>
+        <v/>
       </c>
     </row>
     <row r="18">
@@ -702,7 +706,7 @@
         <v>JP</v>
       </c>
       <c r="E18" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VMAX-Climax/Duraludon-VMAX-V3-s8b285</v>
+        <v/>
       </c>
     </row>
     <row r="19">
@@ -719,7 +723,7 @@
         <v>JP</v>
       </c>
       <c r="E19" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VMAX-Climax/Centiskorch-V-V1-s8b022</v>
+        <v/>
       </c>
     </row>
     <row r="20">
@@ -736,7 +740,7 @@
         <v>JP</v>
       </c>
       <c r="E20" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VMAX-Climax/Umbreon-V-V1-s8b100</v>
+        <v/>
       </c>
     </row>
     <row r="21">
@@ -753,7 +757,7 @@
         <v>JP</v>
       </c>
       <c r="E21" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VMAX-Climax/Zeraora-V-V1-s8b054</v>
+        <v/>
       </c>
     </row>
     <row r="22">
@@ -770,7 +774,7 @@
         <v>JP</v>
       </c>
       <c r="E22" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VMAX-Climax/Galarian-Moltres-V-V1-s8b096</v>
+        <v/>
       </c>
     </row>
     <row r="23">
@@ -787,7 +791,7 @@
         <v>JP</v>
       </c>
       <c r="E23" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VMAX-Climax/Duraludon-V</v>
+        <v/>
       </c>
     </row>
     <row r="24">
@@ -804,7 +808,7 @@
         <v>JP</v>
       </c>
       <c r="E24" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VMAX-Climax/Mimikyu-V-V1-s8b076</v>
+        <v/>
       </c>
     </row>
     <row r="25">
@@ -821,7 +825,7 @@
         <v>JP</v>
       </c>
       <c r="E25" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VMAX-Climax/Rayquaza-VMAX-V1-s8b120</v>
+        <v/>
       </c>
     </row>
     <row r="26">
@@ -838,7 +842,7 @@
         <v>JP</v>
       </c>
       <c r="E26" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VMAX-Climax/Pikachu-VMAX-V1-s8b046</v>
+        <v/>
       </c>
     </row>
     <row r="27">
@@ -855,7 +859,7 @@
         <v>JP</v>
       </c>
       <c r="E27" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VMAX-Climax/Ice-Rider-Calyrex-VMAX-V1-s8b044</v>
+        <v/>
       </c>
     </row>
     <row r="28">
@@ -872,7 +876,7 @@
         <v>JP</v>
       </c>
       <c r="E28" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VMAX-Climax/Flareon-V2-s8b188</v>
+        <v/>
       </c>
     </row>
     <row r="29">
@@ -889,7 +893,7 @@
         <v>JP</v>
       </c>
       <c r="E29" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VMAX-Climax/Eevee-V2-s8b210</v>
+        <v/>
       </c>
     </row>
     <row r="30">
@@ -906,7 +910,7 @@
         <v>JP</v>
       </c>
       <c r="E30" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VMAX-Climax/Falinks-V1-s8b089</v>
+        <v/>
       </c>
     </row>
     <row r="31">
@@ -923,7 +927,7 @@
         <v>JP</v>
       </c>
       <c r="E31" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VMAX-Climax/Corviknight-V-V2-s8b248</v>
+        <v/>
       </c>
     </row>
     <row r="32">
@@ -940,7 +944,7 @@
         <v>JP</v>
       </c>
       <c r="E32" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Machamp-V-s12a071</v>
+        <v/>
       </c>
     </row>
     <row r="33">
@@ -957,7 +961,7 @@
         <v>JP</v>
       </c>
       <c r="E33" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Enamorus-V-s12a068</v>
+        <v/>
       </c>
     </row>
     <row r="34">
@@ -974,7 +978,7 @@
         <v>JP</v>
       </c>
       <c r="E34" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Wyrdeer-V-s12a131</v>
+        <v/>
       </c>
     </row>
     <row r="35">
@@ -991,7 +995,7 @@
         <v>JP</v>
       </c>
       <c r="E35" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Regigigas-V-s12a124</v>
+        <v/>
       </c>
     </row>
     <row r="36">
@@ -1008,7 +1012,7 @@
         <v>JP</v>
       </c>
       <c r="E36" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Mewtwo-V-s12a050</v>
+        <v/>
       </c>
     </row>
     <row r="37">
@@ -1025,7 +1029,7 @@
         <v>JP</v>
       </c>
       <c r="E37" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Comfey-V2-s12a187</v>
+        <v/>
       </c>
     </row>
     <row r="38">
@@ -1042,7 +1046,7 @@
         <v>JP</v>
       </c>
       <c r="E38" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Oricorio-V2-s12a176</v>
+        <v/>
       </c>
     </row>
     <row r="39">
@@ -1059,7 +1063,7 @@
         <v>JP</v>
       </c>
       <c r="E39" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Bibarel-V2-s12a200</v>
+        <v/>
       </c>
     </row>
     <row r="40">
@@ -1076,7 +1080,7 @@
         <v>JP</v>
       </c>
       <c r="E40" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Lightning-Energy-s12a254</v>
+        <v/>
       </c>
     </row>
     <row r="41">
@@ -1093,7 +1097,7 @@
         <v>JP</v>
       </c>
       <c r="E41" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Origin-Forme-Dialga-VSTAR-V1-s12a101</v>
+        <v/>
       </c>
     </row>
     <row r="42">
@@ -1110,7 +1114,7 @@
         <v>JP</v>
       </c>
       <c r="E42" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Giratina-VSTAR-V1-s12a111</v>
+        <v/>
       </c>
     </row>
     <row r="43">
@@ -1127,7 +1131,7 @@
         <v>JP</v>
       </c>
       <c r="E43" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Mew-VMAX-s12a054</v>
+        <v/>
       </c>
     </row>
     <row r="44">
@@ -1144,7 +1148,7 @@
         <v>JP</v>
       </c>
       <c r="E44" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Regigigas-VSTAR-V1-s12a125</v>
+        <v/>
       </c>
     </row>
     <row r="45">
@@ -1161,7 +1165,7 @@
         <v>JP</v>
       </c>
       <c r="E45" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Gardenias-Vigor-V2-s12a243</v>
+        <v/>
       </c>
     </row>
     <row r="46">
@@ -1178,7 +1182,7 @@
         <v>JP</v>
       </c>
       <c r="E46" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Zacian-V-V2-s12a225</v>
+        <v/>
       </c>
     </row>
     <row r="47">
@@ -1195,7 +1199,7 @@
         <v>JP</v>
       </c>
       <c r="E47" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Radiant-Charizard-s12a015</v>
+        <v/>
       </c>
     </row>
     <row r="48">
@@ -1212,7 +1216,7 @@
         <v>JP</v>
       </c>
       <c r="E48" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Entei-V-V2-s12a213</v>
+        <v/>
       </c>
     </row>
     <row r="49">
@@ -1229,7 +1233,7 @@
         <v>JP</v>
       </c>
       <c r="E49" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Rayquaza-VMAX-s12a108</v>
+        <v/>
       </c>
     </row>
     <row r="50">
@@ -1246,7 +1250,7 @@
         <v>JP</v>
       </c>
       <c r="E50" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Origin-Forme-Palkia-VSTAR-V1-s12a028</v>
+        <v/>
       </c>
     </row>
     <row r="51">
@@ -1263,7 +1267,7 @@
         <v>JP</v>
       </c>
       <c r="E51" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Origin-Forme-Dialga-VSTAR-V1-s12a101</v>
+        <v/>
       </c>
     </row>
     <row r="52">
@@ -1280,7 +1284,7 @@
         <v>JP</v>
       </c>
       <c r="E52" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Thievul-V2-s12a192</v>
+        <v/>
       </c>
     </row>
     <row r="53">
@@ -1297,7 +1301,7 @@
         <v>JP</v>
       </c>
       <c r="E53" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Toxtricity-V2-s12a181</v>
+        <v/>
       </c>
     </row>
     <row r="54">
@@ -1314,7 +1318,7 @@
         <v>JP</v>
       </c>
       <c r="E54" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Miltank-V2-s12a199</v>
+        <v/>
       </c>
     </row>
     <row r="55">
@@ -1331,7 +1335,7 @@
         <v>JP</v>
       </c>
       <c r="E55" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Hisuian-Zoroark-V-s12a128</v>
+        <v/>
       </c>
     </row>
     <row r="56">
@@ -1348,7 +1352,7 @@
         <v>JP</v>
       </c>
       <c r="E56" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Zeraora-V-s12a040</v>
+        <v/>
       </c>
     </row>
     <row r="57">
@@ -1365,7 +1369,7 @@
         <v>JP</v>
       </c>
       <c r="E57" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Giratina-V-s12a110</v>
+        <v/>
       </c>
     </row>
     <row r="58">
@@ -1382,7 +1386,7 @@
         <v>JP</v>
       </c>
       <c r="E58" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Hatterene-V-s12a065</v>
+        <v/>
       </c>
     </row>
     <row r="59">
@@ -1399,7 +1403,7 @@
         <v>JP</v>
       </c>
       <c r="E59" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Garchomp-V-s12a109</v>
+        <v/>
       </c>
     </row>
     <row r="60">
@@ -1416,7 +1420,7 @@
         <v>JP</v>
       </c>
       <c r="E60" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Professors-Research-V2-s12a248</v>
+        <v/>
       </c>
     </row>
     <row r="61">
@@ -1433,7 +1437,7 @@
         <v>JP</v>
       </c>
       <c r="E61" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Psychic-Energy-s12a255</v>
+        <v/>
       </c>
     </row>
     <row r="62">
@@ -1450,7 +1454,7 @@
         <v>JP</v>
       </c>
       <c r="E62" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Radiant-Hawlucha-s12a078</v>
+        <v/>
       </c>
     </row>
     <row r="63">
@@ -1467,7 +1471,7 @@
         <v>FR</v>
       </c>
       <c r="E63" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Platinum/Giratina-Lv63-PL10</v>
+        <v/>
       </c>
     </row>
     <row r="64">
@@ -1484,7 +1488,7 @@
         <v>JP</v>
       </c>
       <c r="E64" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Giratina-VSTAR-V2-s12a261</v>
+        <v/>
       </c>
     </row>
     <row r="65">
@@ -1501,7 +1505,7 @@
         <v>JP</v>
       </c>
       <c r="E65" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Darkness-Energy-s12a257</v>
+        <v/>
       </c>
     </row>
     <row r="66">
@@ -1518,7 +1522,7 @@
         <v>JP</v>
       </c>
       <c r="E66" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Metal-Energy-s12a258</v>
+        <v/>
       </c>
     </row>
     <row r="67">
@@ -1535,7 +1539,7 @@
         <v>JP</v>
       </c>
       <c r="E67" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Fire-Energy-s12a252</v>
+        <v/>
       </c>
     </row>
     <row r="68">
@@ -1552,7 +1556,7 @@
         <v>JP</v>
       </c>
       <c r="E68" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Regigigas-VSTAR-V2-s12a233</v>
+        <v/>
       </c>
     </row>
     <row r="69">
@@ -1569,7 +1573,7 @@
         <v>JP</v>
       </c>
       <c r="E69" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Entei-V-V2-s12a213</v>
+        <v/>
       </c>
     </row>
     <row r="70">
@@ -1586,7 +1590,7 @@
         <v>JP</v>
       </c>
       <c r="E70" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Suicune-V-V2-s12a215</v>
+        <v/>
       </c>
     </row>
     <row r="71">
@@ -1603,7 +1607,7 @@
         <v>JP</v>
       </c>
       <c r="E71" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Hisuian-Samurott-V-V2-s12a229</v>
+        <v/>
       </c>
     </row>
     <row r="72">
@@ -1620,7 +1624,7 @@
         <v>JP</v>
       </c>
       <c r="E72" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Darkrai-VSTAR-s12a228</v>
+        <v/>
       </c>
     </row>
     <row r="73">
@@ -1637,7 +1641,7 @@
         <v>JP</v>
       </c>
       <c r="E73" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Deoxys-VMAX-s12a222</v>
+        <v/>
       </c>
     </row>
     <row r="74">
@@ -1654,7 +1658,7 @@
         <v>JP</v>
       </c>
       <c r="E74" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Zacian-V-V2-s12a225</v>
+        <v/>
       </c>
     </row>
     <row r="75">
@@ -1671,7 +1675,7 @@
         <v>JP</v>
       </c>
       <c r="E75" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Hoopa-V-s12a231</v>
+        <v/>
       </c>
     </row>
     <row r="76">
@@ -1688,7 +1692,7 @@
         <v>JP</v>
       </c>
       <c r="E76" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Hisuian-Samurott-VSTAR-V2-s12a230</v>
+        <v/>
       </c>
     </row>
     <row r="77">
@@ -1705,7 +1709,7 @@
         <v>JP</v>
       </c>
       <c r="E77" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Raikou-V-V2-s12a218</v>
+        <v/>
       </c>
     </row>
     <row r="78">
@@ -1722,7 +1726,7 @@
         <v>JP</v>
       </c>
       <c r="E78" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Drapion-V-V2-s12a227</v>
+        <v/>
       </c>
     </row>
     <row r="79">
@@ -1739,7 +1743,7 @@
         <v>JP</v>
       </c>
       <c r="E79" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Keldeo-V2-s12a179</v>
+        <v/>
       </c>
     </row>
     <row r="80">
@@ -1756,7 +1760,7 @@
         <v>JP</v>
       </c>
       <c r="E80" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Dunsparce-V2-s12a198</v>
+        <v/>
       </c>
     </row>
     <row r="81">
@@ -1773,7 +1777,7 @@
         <v>JP</v>
       </c>
       <c r="E81" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Magmortar-V2-s12a175</v>
+        <v/>
       </c>
     </row>
     <row r="82">
@@ -1790,7 +1794,7 @@
         <v>JP</v>
       </c>
       <c r="E82" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Lapras-V2-s12a177</v>
+        <v/>
       </c>
     </row>
     <row r="83">
@@ -1807,7 +1811,7 @@
         <v>JP</v>
       </c>
       <c r="E83" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Electivire-V2-s12a180</v>
+        <v/>
       </c>
     </row>
     <row r="84">
@@ -1824,7 +1828,7 @@
         <v>JP</v>
       </c>
       <c r="E84" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Lunatone-V2-s12a184</v>
+        <v/>
       </c>
     </row>
     <row r="85">
@@ -1841,7 +1845,7 @@
         <v>JP</v>
       </c>
       <c r="E85" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Galarian-Zapdos-V2-s12a188</v>
+        <v/>
       </c>
     </row>
     <row r="86">
@@ -1858,7 +1862,7 @@
         <v>JP</v>
       </c>
       <c r="E86" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Absol-V2-s12a191</v>
+        <v/>
       </c>
     </row>
     <row r="87">
@@ -1875,7 +1879,7 @@
         <v>JP</v>
       </c>
       <c r="E87" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Thievul-V2-s12a192</v>
+        <v/>
       </c>
     </row>
     <row r="88">
@@ -1892,7 +1896,7 @@
         <v>JP</v>
       </c>
       <c r="E88" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Magnezone-V2-s12a193</v>
+        <v/>
       </c>
     </row>
     <row r="89">
@@ -1909,7 +1913,7 @@
         <v>JP</v>
       </c>
       <c r="E89" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Hisuian-Voltorb-V2-s12a173</v>
+        <v/>
       </c>
     </row>
     <row r="90">
@@ -1926,7 +1930,7 @@
         <v>JP</v>
       </c>
       <c r="E90" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Altaria-V2-s12a194</v>
+        <v/>
       </c>
     </row>
     <row r="91">
@@ -1943,7 +1947,7 @@
         <v>JP</v>
       </c>
       <c r="E91" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Mew-V2-s12a183</v>
+        <v/>
       </c>
     </row>
     <row r="92">
@@ -1960,7 +1964,7 @@
         <v>JP</v>
       </c>
       <c r="E92" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Kricketune-V2-s12a174</v>
+        <v/>
       </c>
     </row>
     <row r="93">
@@ -1977,7 +1981,7 @@
         <v>JP</v>
       </c>
       <c r="E93" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Diancie-V2-s12a186</v>
+        <v/>
       </c>
     </row>
     <row r="94">
@@ -1994,7 +1998,7 @@
         <v>JP</v>
       </c>
       <c r="E94" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Galarian-Moltres-V2-s12a190</v>
+        <v/>
       </c>
     </row>
     <row r="95">
@@ -2011,7 +2015,7 @@
         <v>JP</v>
       </c>
       <c r="E95" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Hisuian-Goodra-V2-s12a196</v>
+        <v/>
       </c>
     </row>
     <row r="96">
@@ -2028,7 +2032,7 @@
         <v>JP</v>
       </c>
       <c r="E96" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Galarian-Articuno-V2-s12a182</v>
+        <v/>
       </c>
     </row>
     <row r="97">
@@ -2045,7 +2049,7 @@
         <v>FR</v>
       </c>
       <c r="E97" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/151/Blastoise-ex-V3-MEW200</v>
+        <v/>
       </c>
     </row>
     <row r="98">
@@ -2062,7 +2066,1688 @@
         <v>FR</v>
       </c>
       <c r="E98" t="str">
-        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/151/Giovannis-Charisma-V3-MEW204</v>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:E98"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E98"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Nom</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Numéro</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Série</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Langue</v>
+      </c>
+      <c r="E1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>Noctali</v>
+      </c>
+      <c r="B2" t="str">
+        <v>85/69</v>
+      </c>
+      <c r="C2" t="str">
+        <v>S6A</v>
+      </c>
+      <c r="D2" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E2" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Eevee-Heroes/Umbreon-V-V3-s6a085?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Givrali</v>
+      </c>
+      <c r="B3" t="str">
+        <v>25/69</v>
+      </c>
+      <c r="C3" t="str">
+        <v>S6A</v>
+      </c>
+      <c r="D3" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E3" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Eevee-Heroes/Glaceon-VMAX-V1?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Nymphali</v>
+      </c>
+      <c r="B4" t="str">
+        <v>41/69</v>
+      </c>
+      <c r="C4" t="str">
+        <v>S6A</v>
+      </c>
+      <c r="D4" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E4" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Eevee-Heroes/Sylveon-VMAX-V1-s6a041?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Nocatli</v>
+      </c>
+      <c r="B5" t="str">
+        <v>48/69</v>
+      </c>
+      <c r="C5" t="str">
+        <v>S6A</v>
+      </c>
+      <c r="D5" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E5" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Eevee-Heroes/Umbreon-VMAX-V1?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>Nymphali</v>
+      </c>
+      <c r="B6" t="str">
+        <v>40/69</v>
+      </c>
+      <c r="C6" t="str">
+        <v>S6A</v>
+      </c>
+      <c r="D6" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E6" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Eevee-Heroes/Sylveon-V-V1?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>Givrali</v>
+      </c>
+      <c r="B7" t="str">
+        <v>24/69</v>
+      </c>
+      <c r="C7" t="str">
+        <v>S6A</v>
+      </c>
+      <c r="D7" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E7" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Eevee-Heroes/Glaceon-V-V1-s6a024?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>Aquali</v>
+      </c>
+      <c r="B8" t="str">
+        <v>15/69</v>
+      </c>
+      <c r="C8" t="str">
+        <v>S6A</v>
+      </c>
+      <c r="D8" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E8" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Eevee-Heroes/Vaporeon-V-V1?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>Phyllali</v>
+      </c>
+      <c r="B9" t="str">
+        <v>002/69</v>
+      </c>
+      <c r="C9" t="str">
+        <v>S6A</v>
+      </c>
+      <c r="D9" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E9" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Eevee-Heroes/Leafeon-V-V1?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>Desseliande</v>
+      </c>
+      <c r="B10" t="str">
+        <v>68/67</v>
+      </c>
+      <c r="C10" t="str">
+        <v>S7R</v>
+      </c>
+      <c r="D10" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E10" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Blue-Sky-Stream/Trevenant-V-V2?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>Léviator</v>
+      </c>
+      <c r="B11" t="str">
+        <v>21/67</v>
+      </c>
+      <c r="C11" t="str">
+        <v>S7R</v>
+      </c>
+      <c r="D11" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E11" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Blue-Sky-Stream/Gyarados-VMAX-V1?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>Rayquaza</v>
+      </c>
+      <c r="B12" t="str">
+        <v>47/67</v>
+      </c>
+      <c r="C12" t="str">
+        <v>S7R</v>
+      </c>
+      <c r="D12" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E12" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Blue-Sky-Stream/Rayquaza-VMAX-V1-s7R047?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v xml:space="preserve">Leviator </v>
+      </c>
+      <c r="B13" t="str">
+        <v>20/67</v>
+      </c>
+      <c r="C13" t="str">
+        <v>S7R</v>
+      </c>
+      <c r="D13" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E13" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Blue-Sky-Stream/Gyarados-V-V1-s7R020?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>Rayquaza</v>
+      </c>
+      <c r="B14" t="str">
+        <v>46/67</v>
+      </c>
+      <c r="C14" t="str">
+        <v>S7R</v>
+      </c>
+      <c r="D14" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E14" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Blue-Sky-Stream/Rayquaza-V-V1?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>Pyrax</v>
+      </c>
+      <c r="B15" t="str">
+        <v>15/67</v>
+      </c>
+      <c r="C15" t="str">
+        <v>S7R</v>
+      </c>
+      <c r="D15" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E15" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Blue-Sky-Stream/Volcarona-V-V1-s7R015?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>Desseliande</v>
+      </c>
+      <c r="B16" t="str">
+        <v>007/67</v>
+      </c>
+      <c r="C16" t="str">
+        <v>S7R</v>
+      </c>
+      <c r="D16" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E16" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Blue-Sky-Stream/Trevenant-V-V1?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>Dracolosse</v>
+      </c>
+      <c r="B17" t="str">
+        <v>42/67</v>
+      </c>
+      <c r="C17" t="str">
+        <v>S7R</v>
+      </c>
+      <c r="D17" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E17" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Blue-Sky-Stream/Dragonite-V-V1?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>Vmax Duralugon</v>
+      </c>
+      <c r="B18" t="str">
+        <v>285/184</v>
+      </c>
+      <c r="C18" t="str">
+        <v>S8B</v>
+      </c>
+      <c r="D18" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E18" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VMAX-Climax/Duraludon-VMAX-V3-s8b285?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>V Scolocendre</v>
+      </c>
+      <c r="B19" t="str">
+        <v>22/184</v>
+      </c>
+      <c r="C19" t="str">
+        <v>S8B</v>
+      </c>
+      <c r="D19" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E19" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VMAX-Climax/Centiskorch-V-V1-s8b022?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>V Noctali</v>
+      </c>
+      <c r="B20" t="str">
+        <v>100/184</v>
+      </c>
+      <c r="C20" t="str">
+        <v>S8B</v>
+      </c>
+      <c r="D20" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E20" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VMAX-Climax/Umbreon-V-V1-s8b100?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>V Zeraora</v>
+      </c>
+      <c r="B21" t="str">
+        <v>54/184</v>
+      </c>
+      <c r="C21" t="str">
+        <v>S8B</v>
+      </c>
+      <c r="D21" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E21" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VMAX-Climax/Zeraora-V-V1-s8b054?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>V Sulfura</v>
+      </c>
+      <c r="B22" t="str">
+        <v>96/184</v>
+      </c>
+      <c r="C22" t="str">
+        <v>S8B</v>
+      </c>
+      <c r="D22" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E22" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VMAX-Climax/Galarian-Moltres-V-V1-s8b096?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v xml:space="preserve">V Duralugon </v>
+      </c>
+      <c r="B23" t="str">
+        <v>122/184</v>
+      </c>
+      <c r="C23" t="str">
+        <v>S8B</v>
+      </c>
+      <c r="D23" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E23" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VMAX-Climax/Duraludon-V?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>V Mimiqui</v>
+      </c>
+      <c r="B24" t="str">
+        <v>76/184</v>
+      </c>
+      <c r="C24" t="str">
+        <v>S8B</v>
+      </c>
+      <c r="D24" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E24" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VMAX-Climax/Mimikyu-V-V1-s8b076?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>Vmax Rayquaza</v>
+      </c>
+      <c r="B25" t="str">
+        <v>120/184</v>
+      </c>
+      <c r="C25" t="str">
+        <v>S8B</v>
+      </c>
+      <c r="D25" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E25" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VMAX-Climax/Rayquaza-VMAX-V1-s8b120?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>Vmax Pikachu</v>
+      </c>
+      <c r="B26" t="str">
+        <v>46/184</v>
+      </c>
+      <c r="C26" t="str">
+        <v>S8B</v>
+      </c>
+      <c r="D26" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E26" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VMAX-Climax/Pikachu-VMAX-V1-s8b046?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v xml:space="preserve">Vmax Sylveroy </v>
+      </c>
+      <c r="B27" t="str">
+        <v>44/184</v>
+      </c>
+      <c r="C27" t="str">
+        <v>S8B</v>
+      </c>
+      <c r="D27" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E27" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VMAX-Climax/Ice-Rider-Calyrex-VMAX-V1-s8b044?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>Pyroli</v>
+      </c>
+      <c r="B28" t="str">
+        <v>188/184</v>
+      </c>
+      <c r="C28" t="str">
+        <v>S8B</v>
+      </c>
+      <c r="D28" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E28" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VMAX-Climax/Flareon-V2-s8b188?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>Evoli</v>
+      </c>
+      <c r="B29" t="str">
+        <v>210/184</v>
+      </c>
+      <c r="C29" t="str">
+        <v>S8B</v>
+      </c>
+      <c r="D29" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E29" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VMAX-Climax/Eevee-V2-s8b210?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>Hexadron</v>
+      </c>
+      <c r="B30" t="str">
+        <v>201/184</v>
+      </c>
+      <c r="C30" t="str">
+        <v>S8B</v>
+      </c>
+      <c r="D30" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E30" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VMAX-Climax/Falinks-V1-s8b089?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>V Corvaillus</v>
+      </c>
+      <c r="B31" t="str">
+        <v>248/184</v>
+      </c>
+      <c r="C31" t="str">
+        <v>S8B</v>
+      </c>
+      <c r="D31" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E31" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VMAX-Climax/Corviknight-V-V2-s8b248?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>V Mackogneur</v>
+      </c>
+      <c r="B32" t="str">
+        <v>71/172</v>
+      </c>
+      <c r="C32" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D32" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E32" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Machamp-V-s12a071?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>V Amovénus</v>
+      </c>
+      <c r="B33" t="str">
+        <v>68/172</v>
+      </c>
+      <c r="C33" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D33" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E33" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Enamorus-V-s12a068?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>V Cerbyllin</v>
+      </c>
+      <c r="B34" t="str">
+        <v>131/172</v>
+      </c>
+      <c r="C34" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D34" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E34" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Wyrdeer-V-s12a131?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>V Regigigas</v>
+      </c>
+      <c r="B35" t="str">
+        <v>124/172</v>
+      </c>
+      <c r="C35" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D35" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E35" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Regigigas-V-s12a124?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>V Mewtwo</v>
+      </c>
+      <c r="B36" t="str">
+        <v>50/172</v>
+      </c>
+      <c r="C36" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D36" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E36" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Mewtwo-V-s12a050?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>Guérilande</v>
+      </c>
+      <c r="B37" t="str">
+        <v>187/172</v>
+      </c>
+      <c r="C37" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D37" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E37" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Comfey-V2-s12a187?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>Plumeline</v>
+      </c>
+      <c r="B38" t="str">
+        <v>176/172</v>
+      </c>
+      <c r="C38" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D38" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E38" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Oricorio-V2-s12a176?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>Castorno</v>
+      </c>
+      <c r="B39" t="str">
+        <v>200/172</v>
+      </c>
+      <c r="C39" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D39" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E39" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Bibarel-V2-s12a200?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>Energie elect</v>
+      </c>
+      <c r="B40" t="str">
+        <v>254/172</v>
+      </c>
+      <c r="C40" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D40" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E40" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Lightning-Energy-s12a254?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>Vstar Dialga</v>
+      </c>
+      <c r="B41" t="str">
+        <v>101/172</v>
+      </c>
+      <c r="C41" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D41" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E41" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Origin-Forme-Dialga-VSTAR-V1-s12a101?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>Vstar Giratina</v>
+      </c>
+      <c r="B42" t="str">
+        <v>111/172</v>
+      </c>
+      <c r="C42" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D42" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E42" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Giratina-VSTAR-V1-s12a111?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>Vmax Mew</v>
+      </c>
+      <c r="B43" t="str">
+        <v>54/172</v>
+      </c>
+      <c r="C43" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D43" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E43" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Mew-VMAX-s12a054?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>Vstar Regigigas</v>
+      </c>
+      <c r="B44" t="str">
+        <v>125/172</v>
+      </c>
+      <c r="C44" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D44" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E44" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Regigigas-VSTAR-V1-s12a125?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>Vitalité de Flo</v>
+      </c>
+      <c r="B45" t="str">
+        <v>243/172</v>
+      </c>
+      <c r="C45" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D45" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E45" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Gardenias-Vigor-V2-s12a243?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v>V Zacian</v>
+      </c>
+      <c r="B46" t="str">
+        <v>225/172</v>
+      </c>
+      <c r="C46" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D46" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E46" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Zacian-V-V2-s12a225?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>Dracaufeu Radieux</v>
+      </c>
+      <c r="B47" t="str">
+        <v>015/172</v>
+      </c>
+      <c r="C47" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D47" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E47" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Radiant-Charizard-s12a015?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v>Entei V</v>
+      </c>
+      <c r="B48" t="str">
+        <v>213/172</v>
+      </c>
+      <c r="C48" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D48" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E48" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Entei-V-V2-s12a213?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="str">
+        <v>Rayquaza VMAX</v>
+      </c>
+      <c r="B49" t="str">
+        <v>108/172</v>
+      </c>
+      <c r="C49" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D49" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E49" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Rayquaza-VMAX-s12a108?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="str">
+        <v>Palkia Originel VSTAR</v>
+      </c>
+      <c r="B50" t="str">
+        <v>028/172</v>
+      </c>
+      <c r="C50" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D50" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E50" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Origin-Forme-Palkia-VSTAR-V1-s12a028?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="str">
+        <v>Dialga Originel VSTAR</v>
+      </c>
+      <c r="B51" t="str">
+        <v>101/172</v>
+      </c>
+      <c r="C51" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D51" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E51" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Origin-Forme-Dialga-VSTAR-V1-s12a101?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="str">
+        <v>Roublenard</v>
+      </c>
+      <c r="B52" t="str">
+        <v>192/172</v>
+      </c>
+      <c r="C52" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D52" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E52" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Thievul-V2-s12a192?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="str">
+        <v>Salarsen</v>
+      </c>
+      <c r="B53" t="str">
+        <v>181/172</v>
+      </c>
+      <c r="C53" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D53" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E53" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Toxtricity-V2-s12a181?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="str">
+        <v>Ecrémeuf</v>
+      </c>
+      <c r="B54" t="str">
+        <v>199/172</v>
+      </c>
+      <c r="C54" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D54" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E54" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Miltank-V2-s12a199?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="str">
+        <v>Zoroark de Hisui V</v>
+      </c>
+      <c r="B55" t="str">
+        <v>128/172</v>
+      </c>
+      <c r="C55" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D55" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E55" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Hisuian-Zoroark-V-s12a128?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="str">
+        <v>Zeraora V</v>
+      </c>
+      <c r="B56" t="str">
+        <v>040/172</v>
+      </c>
+      <c r="C56" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D56" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E56" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Zeraora-V-s12a040?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="str">
+        <v>Giratina V</v>
+      </c>
+      <c r="B57" t="str">
+        <v>110/172</v>
+      </c>
+      <c r="C57" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D57" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E57" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Giratina-V-s12a110?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="str">
+        <v>Sorcilence</v>
+      </c>
+      <c r="B58" t="str">
+        <v>065/172</v>
+      </c>
+      <c r="C58" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D58" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E58" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Hatterene-V-s12a065?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="str">
+        <v>Carchacrock V</v>
+      </c>
+      <c r="B59" t="str">
+        <v>109/172</v>
+      </c>
+      <c r="C59" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D59" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E59" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Garchomp-V-s12a109?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="str">
+        <v>Recherche Professorale</v>
+      </c>
+      <c r="B60" t="str">
+        <v>248/172</v>
+      </c>
+      <c r="C60" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D60" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E60" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Professors-Research-V2-s12a248?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="str">
+        <v>Energie Psy</v>
+      </c>
+      <c r="B61" t="str">
+        <v>255/172</v>
+      </c>
+      <c r="C61" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D61" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E61" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Psychic-Energy-s12a255?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="str">
+        <v>Brutalibré Radieux</v>
+      </c>
+      <c r="B62" t="str">
+        <v>078/172</v>
+      </c>
+      <c r="C62" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D62" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E62" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Radiant-Hawlucha-s12a078?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="str">
+        <v>Giratina Holo</v>
+      </c>
+      <c r="B63" t="str">
+        <v>10/127</v>
+      </c>
+      <c r="C63" t="str">
+        <v>Platine</v>
+      </c>
+      <c r="D63" t="str">
+        <v>FR</v>
+      </c>
+      <c r="E63" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Platinum/Giratina-Lv63-PL10?language=2&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="str">
+        <v>Giratina VSTAR</v>
+      </c>
+      <c r="B64" t="str">
+        <v>261/172</v>
+      </c>
+      <c r="C64" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D64" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E64" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Giratina-VSTAR-V2-s12a261?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="str">
+        <v>Energie Tênebre</v>
+      </c>
+      <c r="B65" t="str">
+        <v>257/172</v>
+      </c>
+      <c r="C65" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D65" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E65" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Darkness-Energy-s12a257?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="str">
+        <v>Energie Acier</v>
+      </c>
+      <c r="B66" t="str">
+        <v>258/172</v>
+      </c>
+      <c r="C66" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D66" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E66" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Metal-Energy-s12a258?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="str">
+        <v>Energie Feu</v>
+      </c>
+      <c r="B67" t="str">
+        <v>252/172</v>
+      </c>
+      <c r="C67" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D67" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E67" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Fire-Energy-s12a252?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="str">
+        <v>Regigigas VSTAR</v>
+      </c>
+      <c r="B68" t="str">
+        <v>233/172</v>
+      </c>
+      <c r="C68" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D68" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E68" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Regigigas-VSTAR-V2-s12a233?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="str">
+        <v>Entei V</v>
+      </c>
+      <c r="B69" t="str">
+        <v>213/172</v>
+      </c>
+      <c r="C69" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D69" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E69" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Entei-V-V2-s12a213?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="str">
+        <v xml:space="preserve">Suicune </v>
+      </c>
+      <c r="B70" t="str">
+        <v>215/172</v>
+      </c>
+      <c r="C70" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D70" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E70" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Suicune-V-V2-s12a215?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="str">
+        <v>Clamiral</v>
+      </c>
+      <c r="B71" t="str">
+        <v>229/172</v>
+      </c>
+      <c r="C71" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D71" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E71" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Hisuian-Samurott-V-V2-s12a229?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="str">
+        <v>Darkrai VSTAR</v>
+      </c>
+      <c r="B72" t="str">
+        <v>228/172</v>
+      </c>
+      <c r="C72" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D72" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E72" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Darkrai-VSTAR-s12a228?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="str">
+        <v>Deoxy Vmax</v>
+      </c>
+      <c r="B73" t="str">
+        <v>222/172</v>
+      </c>
+      <c r="C73" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D73" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E73" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Deoxys-VMAX-s12a222?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="str">
+        <v>Zacian V</v>
+      </c>
+      <c r="B74" t="str">
+        <v>225/172</v>
+      </c>
+      <c r="C74" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D74" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E74" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Zacian-V-V2-s12a225?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="str">
+        <v>Hoopa</v>
+      </c>
+      <c r="B75" t="str">
+        <v>231/172</v>
+      </c>
+      <c r="C75" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D75" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E75" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Hoopa-V-s12a231?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="str">
+        <v>Clamiral Vstar</v>
+      </c>
+      <c r="B76" t="str">
+        <v>230/172</v>
+      </c>
+      <c r="C76" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D76" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E76" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Hisuian-Samurott-VSTAR-V2-s12a230?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="str">
+        <v>Raikou</v>
+      </c>
+      <c r="B77" t="str">
+        <v>218/172</v>
+      </c>
+      <c r="C77" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D77" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E77" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Raikou-V-V2-s12a218?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="str">
+        <v>Drascore</v>
+      </c>
+      <c r="B78" t="str">
+        <v>227/172</v>
+      </c>
+      <c r="C78" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D78" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E78" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Drapion-V-V2-s12a227?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="str">
+        <v>Keldeo</v>
+      </c>
+      <c r="B79" t="str">
+        <v>179/172</v>
+      </c>
+      <c r="C79" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D79" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E79" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Keldeo-V2-s12a179?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="str">
+        <v>Insolourdo</v>
+      </c>
+      <c r="B80" t="str">
+        <v>198/172</v>
+      </c>
+      <c r="C80" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D80" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E80" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Dunsparce-V2-s12a198?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="str">
+        <v>Maganon</v>
+      </c>
+      <c r="B81" t="str">
+        <v>175/172</v>
+      </c>
+      <c r="C81" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D81" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E81" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Magmortar-V2-s12a175?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="str">
+        <v>Locklass</v>
+      </c>
+      <c r="B82" t="str">
+        <v>177/172</v>
+      </c>
+      <c r="C82" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D82" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E82" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Lapras-V2-s12a177?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="str">
+        <v>Elekable</v>
+      </c>
+      <c r="B83" t="str">
+        <v>180/172</v>
+      </c>
+      <c r="C83" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D83" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E83" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Electivire-V2-s12a180?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="str">
+        <v>Séléroc</v>
+      </c>
+      <c r="B84" t="str">
+        <v>184/172</v>
+      </c>
+      <c r="C84" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D84" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E84" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Lunatone-V2-s12a184?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="str">
+        <v>Electhor de Galar</v>
+      </c>
+      <c r="B85" t="str">
+        <v>188/172</v>
+      </c>
+      <c r="C85" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D85" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E85" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Galarian-Zapdos-V2-s12a188?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="str">
+        <v>Absol</v>
+      </c>
+      <c r="B86" t="str">
+        <v>191/172</v>
+      </c>
+      <c r="C86" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D86" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E86" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Absol-V2-s12a191?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="str">
+        <v>Roublenard</v>
+      </c>
+      <c r="B87" t="str">
+        <v>192/172</v>
+      </c>
+      <c r="C87" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D87" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E87" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Thievul-V2-s12a192?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="str">
+        <v>Magnézone</v>
+      </c>
+      <c r="B88" t="str">
+        <v>193/172</v>
+      </c>
+      <c r="C88" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D88" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E88" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Magnezone-V2-s12a193?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="str">
+        <v>Voltorbe de Hisui</v>
+      </c>
+      <c r="B89" t="str">
+        <v>173/172</v>
+      </c>
+      <c r="C89" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D89" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E89" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Hisuian-Voltorb-V2-s12a173?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="str">
+        <v>Altaria</v>
+      </c>
+      <c r="B90" t="str">
+        <v>194/172</v>
+      </c>
+      <c r="C90" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D90" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E90" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Altaria-V2-s12a194?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="str">
+        <v>Mew</v>
+      </c>
+      <c r="B91" t="str">
+        <v>183/172</v>
+      </c>
+      <c r="C91" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D91" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E91" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Mew-V2-s12a183?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="str">
+        <v>Melokrik</v>
+      </c>
+      <c r="B92" t="str">
+        <v>174/172</v>
+      </c>
+      <c r="C92" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D92" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E92" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Kricketune-V2-s12a174?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="str">
+        <v>Diancy</v>
+      </c>
+      <c r="B93" t="str">
+        <v>186/172</v>
+      </c>
+      <c r="C93" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D93" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E93" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Diancie-V2-s12a186?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="str">
+        <v>Sulfura Galar</v>
+      </c>
+      <c r="B94" t="str">
+        <v>190/172</v>
+      </c>
+      <c r="C94" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D94" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E94" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Galarian-Moltres-V2-s12a190?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="str">
+        <v>Muplodocus</v>
+      </c>
+      <c r="B95" t="str">
+        <v>196/172</v>
+      </c>
+      <c r="C95" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D95" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E95" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Hisuian-Goodra-V2-s12a196?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="str">
+        <v>Artikodin Galar</v>
+      </c>
+      <c r="B96" t="str">
+        <v>182/172</v>
+      </c>
+      <c r="C96" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D96" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E96" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Galarian-Articuno-V2-s12a182?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="str">
+        <v>Tortank Ex</v>
+      </c>
+      <c r="B97" t="str">
+        <v>200/165</v>
+      </c>
+      <c r="C97">
+        <v>151</v>
+      </c>
+      <c r="D97" t="str">
+        <v>FR</v>
+      </c>
+      <c r="E97" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/151/Blastoise-ex-V3-MEW200?language=2&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="str">
+        <v>Charisme de Giovanni</v>
+      </c>
+      <c r="B98" t="str">
+        <v>204/165</v>
+      </c>
+      <c r="C98">
+        <v>151</v>
+      </c>
+      <c r="D98" t="str">
+        <v>FR</v>
+      </c>
+      <c r="E98" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/151/Giovannis-Charisma-V3-MEW204?language=2&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updateXlsxWithCardsUrl update -> create new xlsx sheet with today date as name, find the cardUrl and add filter to it in E column, when no E column in the first sheet, create it in the second -> tests ok
</commit_message>
<xml_diff>
--- a/excelPriceCards/cartes.xlsx
+++ b/excelPriceCards/cartes.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E98"/>
+  <dimension ref="A1:D98"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -416,9 +416,6 @@
       <c r="D1" t="str">
         <v>Langue</v>
       </c>
-      <c r="E1" t="str">
-        <v/>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -433,9 +430,6 @@
       <c r="D2" t="str">
         <v>JP</v>
       </c>
-      <c r="E2" t="str">
-        <v/>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -450,9 +444,6 @@
       <c r="D3" t="str">
         <v>JP</v>
       </c>
-      <c r="E3" t="str">
-        <v/>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
@@ -467,9 +458,6 @@
       <c r="D4" t="str">
         <v>JP</v>
       </c>
-      <c r="E4" t="str">
-        <v/>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
@@ -484,9 +472,6 @@
       <c r="D5" t="str">
         <v>JP</v>
       </c>
-      <c r="E5" t="str">
-        <v/>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
@@ -501,9 +486,6 @@
       <c r="D6" t="str">
         <v>JP</v>
       </c>
-      <c r="E6" t="str">
-        <v/>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
@@ -518,9 +500,6 @@
       <c r="D7" t="str">
         <v>JP</v>
       </c>
-      <c r="E7" t="str">
-        <v/>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
@@ -535,9 +514,6 @@
       <c r="D8" t="str">
         <v>JP</v>
       </c>
-      <c r="E8" t="str">
-        <v/>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
@@ -552,9 +528,6 @@
       <c r="D9" t="str">
         <v>JP</v>
       </c>
-      <c r="E9" t="str">
-        <v/>
-      </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
@@ -569,9 +542,6 @@
       <c r="D10" t="str">
         <v>JP</v>
       </c>
-      <c r="E10" t="str">
-        <v/>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
@@ -586,9 +556,6 @@
       <c r="D11" t="str">
         <v>JP</v>
       </c>
-      <c r="E11" t="str">
-        <v/>
-      </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
@@ -603,9 +570,6 @@
       <c r="D12" t="str">
         <v>JP</v>
       </c>
-      <c r="E12" t="str">
-        <v/>
-      </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
@@ -620,9 +584,6 @@
       <c r="D13" t="str">
         <v>JP</v>
       </c>
-      <c r="E13" t="str">
-        <v/>
-      </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
@@ -637,9 +598,6 @@
       <c r="D14" t="str">
         <v>JP</v>
       </c>
-      <c r="E14" t="str">
-        <v/>
-      </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
@@ -654,9 +612,6 @@
       <c r="D15" t="str">
         <v>JP</v>
       </c>
-      <c r="E15" t="str">
-        <v/>
-      </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
@@ -671,9 +626,6 @@
       <c r="D16" t="str">
         <v>JP</v>
       </c>
-      <c r="E16" t="str">
-        <v/>
-      </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
@@ -688,9 +640,6 @@
       <c r="D17" t="str">
         <v>JP</v>
       </c>
-      <c r="E17" t="str">
-        <v/>
-      </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
@@ -705,9 +654,6 @@
       <c r="D18" t="str">
         <v>JP</v>
       </c>
-      <c r="E18" t="str">
-        <v/>
-      </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
@@ -722,9 +668,6 @@
       <c r="D19" t="str">
         <v>JP</v>
       </c>
-      <c r="E19" t="str">
-        <v/>
-      </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
@@ -739,9 +682,6 @@
       <c r="D20" t="str">
         <v>JP</v>
       </c>
-      <c r="E20" t="str">
-        <v/>
-      </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
@@ -756,9 +696,6 @@
       <c r="D21" t="str">
         <v>JP</v>
       </c>
-      <c r="E21" t="str">
-        <v/>
-      </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
@@ -773,9 +710,6 @@
       <c r="D22" t="str">
         <v>JP</v>
       </c>
-      <c r="E22" t="str">
-        <v/>
-      </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
@@ -790,9 +724,6 @@
       <c r="D23" t="str">
         <v>JP</v>
       </c>
-      <c r="E23" t="str">
-        <v/>
-      </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
@@ -807,9 +738,6 @@
       <c r="D24" t="str">
         <v>JP</v>
       </c>
-      <c r="E24" t="str">
-        <v/>
-      </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
@@ -824,9 +752,6 @@
       <c r="D25" t="str">
         <v>JP</v>
       </c>
-      <c r="E25" t="str">
-        <v/>
-      </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
@@ -841,9 +766,6 @@
       <c r="D26" t="str">
         <v>JP</v>
       </c>
-      <c r="E26" t="str">
-        <v/>
-      </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
@@ -858,9 +780,6 @@
       <c r="D27" t="str">
         <v>JP</v>
       </c>
-      <c r="E27" t="str">
-        <v/>
-      </c>
     </row>
     <row r="28">
       <c r="A28" t="str">
@@ -875,9 +794,6 @@
       <c r="D28" t="str">
         <v>JP</v>
       </c>
-      <c r="E28" t="str">
-        <v/>
-      </c>
     </row>
     <row r="29">
       <c r="A29" t="str">
@@ -892,9 +808,6 @@
       <c r="D29" t="str">
         <v>JP</v>
       </c>
-      <c r="E29" t="str">
-        <v/>
-      </c>
     </row>
     <row r="30">
       <c r="A30" t="str">
@@ -909,9 +822,6 @@
       <c r="D30" t="str">
         <v>JP</v>
       </c>
-      <c r="E30" t="str">
-        <v/>
-      </c>
     </row>
     <row r="31">
       <c r="A31" t="str">
@@ -926,9 +836,6 @@
       <c r="D31" t="str">
         <v>JP</v>
       </c>
-      <c r="E31" t="str">
-        <v/>
-      </c>
     </row>
     <row r="32">
       <c r="A32" t="str">
@@ -943,9 +850,6 @@
       <c r="D32" t="str">
         <v>JP</v>
       </c>
-      <c r="E32" t="str">
-        <v/>
-      </c>
     </row>
     <row r="33">
       <c r="A33" t="str">
@@ -960,9 +864,6 @@
       <c r="D33" t="str">
         <v>JP</v>
       </c>
-      <c r="E33" t="str">
-        <v/>
-      </c>
     </row>
     <row r="34">
       <c r="A34" t="str">
@@ -977,9 +878,6 @@
       <c r="D34" t="str">
         <v>JP</v>
       </c>
-      <c r="E34" t="str">
-        <v/>
-      </c>
     </row>
     <row r="35">
       <c r="A35" t="str">
@@ -994,9 +892,6 @@
       <c r="D35" t="str">
         <v>JP</v>
       </c>
-      <c r="E35" t="str">
-        <v/>
-      </c>
     </row>
     <row r="36">
       <c r="A36" t="str">
@@ -1011,9 +906,6 @@
       <c r="D36" t="str">
         <v>JP</v>
       </c>
-      <c r="E36" t="str">
-        <v/>
-      </c>
     </row>
     <row r="37">
       <c r="A37" t="str">
@@ -1028,9 +920,6 @@
       <c r="D37" t="str">
         <v>JP</v>
       </c>
-      <c r="E37" t="str">
-        <v/>
-      </c>
     </row>
     <row r="38">
       <c r="A38" t="str">
@@ -1045,9 +934,6 @@
       <c r="D38" t="str">
         <v>JP</v>
       </c>
-      <c r="E38" t="str">
-        <v/>
-      </c>
     </row>
     <row r="39">
       <c r="A39" t="str">
@@ -1062,9 +948,6 @@
       <c r="D39" t="str">
         <v>JP</v>
       </c>
-      <c r="E39" t="str">
-        <v/>
-      </c>
     </row>
     <row r="40">
       <c r="A40" t="str">
@@ -1079,9 +962,6 @@
       <c r="D40" t="str">
         <v>JP</v>
       </c>
-      <c r="E40" t="str">
-        <v/>
-      </c>
     </row>
     <row r="41">
       <c r="A41" t="str">
@@ -1096,9 +976,6 @@
       <c r="D41" t="str">
         <v>JP</v>
       </c>
-      <c r="E41" t="str">
-        <v/>
-      </c>
     </row>
     <row r="42">
       <c r="A42" t="str">
@@ -1113,9 +990,6 @@
       <c r="D42" t="str">
         <v>JP</v>
       </c>
-      <c r="E42" t="str">
-        <v/>
-      </c>
     </row>
     <row r="43">
       <c r="A43" t="str">
@@ -1130,9 +1004,6 @@
       <c r="D43" t="str">
         <v>JP</v>
       </c>
-      <c r="E43" t="str">
-        <v/>
-      </c>
     </row>
     <row r="44">
       <c r="A44" t="str">
@@ -1147,9 +1018,6 @@
       <c r="D44" t="str">
         <v>JP</v>
       </c>
-      <c r="E44" t="str">
-        <v/>
-      </c>
     </row>
     <row r="45">
       <c r="A45" t="str">
@@ -1164,9 +1032,6 @@
       <c r="D45" t="str">
         <v>JP</v>
       </c>
-      <c r="E45" t="str">
-        <v/>
-      </c>
     </row>
     <row r="46">
       <c r="A46" t="str">
@@ -1181,9 +1046,6 @@
       <c r="D46" t="str">
         <v>JP</v>
       </c>
-      <c r="E46" t="str">
-        <v/>
-      </c>
     </row>
     <row r="47">
       <c r="A47" t="str">
@@ -1198,9 +1060,6 @@
       <c r="D47" t="str">
         <v>JP</v>
       </c>
-      <c r="E47" t="str">
-        <v/>
-      </c>
     </row>
     <row r="48">
       <c r="A48" t="str">
@@ -1215,9 +1074,6 @@
       <c r="D48" t="str">
         <v>JP</v>
       </c>
-      <c r="E48" t="str">
-        <v/>
-      </c>
     </row>
     <row r="49">
       <c r="A49" t="str">
@@ -1232,9 +1088,6 @@
       <c r="D49" t="str">
         <v>JP</v>
       </c>
-      <c r="E49" t="str">
-        <v/>
-      </c>
     </row>
     <row r="50">
       <c r="A50" t="str">
@@ -1249,9 +1102,6 @@
       <c r="D50" t="str">
         <v>JP</v>
       </c>
-      <c r="E50" t="str">
-        <v/>
-      </c>
     </row>
     <row r="51">
       <c r="A51" t="str">
@@ -1266,9 +1116,6 @@
       <c r="D51" t="str">
         <v>JP</v>
       </c>
-      <c r="E51" t="str">
-        <v/>
-      </c>
     </row>
     <row r="52">
       <c r="A52" t="str">
@@ -1283,9 +1130,6 @@
       <c r="D52" t="str">
         <v>JP</v>
       </c>
-      <c r="E52" t="str">
-        <v/>
-      </c>
     </row>
     <row r="53">
       <c r="A53" t="str">
@@ -1300,9 +1144,6 @@
       <c r="D53" t="str">
         <v>JP</v>
       </c>
-      <c r="E53" t="str">
-        <v/>
-      </c>
     </row>
     <row r="54">
       <c r="A54" t="str">
@@ -1317,9 +1158,6 @@
       <c r="D54" t="str">
         <v>JP</v>
       </c>
-      <c r="E54" t="str">
-        <v/>
-      </c>
     </row>
     <row r="55">
       <c r="A55" t="str">
@@ -1334,9 +1172,6 @@
       <c r="D55" t="str">
         <v>JP</v>
       </c>
-      <c r="E55" t="str">
-        <v/>
-      </c>
     </row>
     <row r="56">
       <c r="A56" t="str">
@@ -1351,9 +1186,6 @@
       <c r="D56" t="str">
         <v>JP</v>
       </c>
-      <c r="E56" t="str">
-        <v/>
-      </c>
     </row>
     <row r="57">
       <c r="A57" t="str">
@@ -1368,9 +1200,6 @@
       <c r="D57" t="str">
         <v>JP</v>
       </c>
-      <c r="E57" t="str">
-        <v/>
-      </c>
     </row>
     <row r="58">
       <c r="A58" t="str">
@@ -1385,9 +1214,6 @@
       <c r="D58" t="str">
         <v>JP</v>
       </c>
-      <c r="E58" t="str">
-        <v/>
-      </c>
     </row>
     <row r="59">
       <c r="A59" t="str">
@@ -1402,9 +1228,6 @@
       <c r="D59" t="str">
         <v>JP</v>
       </c>
-      <c r="E59" t="str">
-        <v/>
-      </c>
     </row>
     <row r="60">
       <c r="A60" t="str">
@@ -1419,9 +1242,6 @@
       <c r="D60" t="str">
         <v>JP</v>
       </c>
-      <c r="E60" t="str">
-        <v/>
-      </c>
     </row>
     <row r="61">
       <c r="A61" t="str">
@@ -1436,9 +1256,6 @@
       <c r="D61" t="str">
         <v>JP</v>
       </c>
-      <c r="E61" t="str">
-        <v/>
-      </c>
     </row>
     <row r="62">
       <c r="A62" t="str">
@@ -1453,9 +1270,6 @@
       <c r="D62" t="str">
         <v>JP</v>
       </c>
-      <c r="E62" t="str">
-        <v/>
-      </c>
     </row>
     <row r="63">
       <c r="A63" t="str">
@@ -1470,9 +1284,6 @@
       <c r="D63" t="str">
         <v>FR</v>
       </c>
-      <c r="E63" t="str">
-        <v/>
-      </c>
     </row>
     <row r="64">
       <c r="A64" t="str">
@@ -1487,9 +1298,6 @@
       <c r="D64" t="str">
         <v>JP</v>
       </c>
-      <c r="E64" t="str">
-        <v/>
-      </c>
     </row>
     <row r="65">
       <c r="A65" t="str">
@@ -1504,9 +1312,6 @@
       <c r="D65" t="str">
         <v>JP</v>
       </c>
-      <c r="E65" t="str">
-        <v/>
-      </c>
     </row>
     <row r="66">
       <c r="A66" t="str">
@@ -1521,9 +1326,6 @@
       <c r="D66" t="str">
         <v>JP</v>
       </c>
-      <c r="E66" t="str">
-        <v/>
-      </c>
     </row>
     <row r="67">
       <c r="A67" t="str">
@@ -1538,9 +1340,6 @@
       <c r="D67" t="str">
         <v>JP</v>
       </c>
-      <c r="E67" t="str">
-        <v/>
-      </c>
     </row>
     <row r="68">
       <c r="A68" t="str">
@@ -1555,9 +1354,6 @@
       <c r="D68" t="str">
         <v>JP</v>
       </c>
-      <c r="E68" t="str">
-        <v/>
-      </c>
     </row>
     <row r="69">
       <c r="A69" t="str">
@@ -1572,9 +1368,6 @@
       <c r="D69" t="str">
         <v>JP</v>
       </c>
-      <c r="E69" t="str">
-        <v/>
-      </c>
     </row>
     <row r="70">
       <c r="A70" t="str">
@@ -1589,9 +1382,6 @@
       <c r="D70" t="str">
         <v>JP</v>
       </c>
-      <c r="E70" t="str">
-        <v/>
-      </c>
     </row>
     <row r="71">
       <c r="A71" t="str">
@@ -1606,9 +1396,6 @@
       <c r="D71" t="str">
         <v>JP</v>
       </c>
-      <c r="E71" t="str">
-        <v/>
-      </c>
     </row>
     <row r="72">
       <c r="A72" t="str">
@@ -1623,9 +1410,6 @@
       <c r="D72" t="str">
         <v>JP</v>
       </c>
-      <c r="E72" t="str">
-        <v/>
-      </c>
     </row>
     <row r="73">
       <c r="A73" t="str">
@@ -1640,9 +1424,6 @@
       <c r="D73" t="str">
         <v>JP</v>
       </c>
-      <c r="E73" t="str">
-        <v/>
-      </c>
     </row>
     <row r="74">
       <c r="A74" t="str">
@@ -1657,9 +1438,6 @@
       <c r="D74" t="str">
         <v>JP</v>
       </c>
-      <c r="E74" t="str">
-        <v/>
-      </c>
     </row>
     <row r="75">
       <c r="A75" t="str">
@@ -1674,9 +1452,6 @@
       <c r="D75" t="str">
         <v>JP</v>
       </c>
-      <c r="E75" t="str">
-        <v/>
-      </c>
     </row>
     <row r="76">
       <c r="A76" t="str">
@@ -1691,9 +1466,6 @@
       <c r="D76" t="str">
         <v>JP</v>
       </c>
-      <c r="E76" t="str">
-        <v/>
-      </c>
     </row>
     <row r="77">
       <c r="A77" t="str">
@@ -1708,9 +1480,6 @@
       <c r="D77" t="str">
         <v>JP</v>
       </c>
-      <c r="E77" t="str">
-        <v/>
-      </c>
     </row>
     <row r="78">
       <c r="A78" t="str">
@@ -1725,9 +1494,6 @@
       <c r="D78" t="str">
         <v>JP</v>
       </c>
-      <c r="E78" t="str">
-        <v/>
-      </c>
     </row>
     <row r="79">
       <c r="A79" t="str">
@@ -1742,9 +1508,6 @@
       <c r="D79" t="str">
         <v>JP</v>
       </c>
-      <c r="E79" t="str">
-        <v/>
-      </c>
     </row>
     <row r="80">
       <c r="A80" t="str">
@@ -1759,9 +1522,6 @@
       <c r="D80" t="str">
         <v>JP</v>
       </c>
-      <c r="E80" t="str">
-        <v/>
-      </c>
     </row>
     <row r="81">
       <c r="A81" t="str">
@@ -1776,9 +1536,6 @@
       <c r="D81" t="str">
         <v>JP</v>
       </c>
-      <c r="E81" t="str">
-        <v/>
-      </c>
     </row>
     <row r="82">
       <c r="A82" t="str">
@@ -1793,9 +1550,6 @@
       <c r="D82" t="str">
         <v>JP</v>
       </c>
-      <c r="E82" t="str">
-        <v/>
-      </c>
     </row>
     <row r="83">
       <c r="A83" t="str">
@@ -1810,9 +1564,6 @@
       <c r="D83" t="str">
         <v>JP</v>
       </c>
-      <c r="E83" t="str">
-        <v/>
-      </c>
     </row>
     <row r="84">
       <c r="A84" t="str">
@@ -1827,9 +1578,6 @@
       <c r="D84" t="str">
         <v>JP</v>
       </c>
-      <c r="E84" t="str">
-        <v/>
-      </c>
     </row>
     <row r="85">
       <c r="A85" t="str">
@@ -1844,9 +1592,6 @@
       <c r="D85" t="str">
         <v>JP</v>
       </c>
-      <c r="E85" t="str">
-        <v/>
-      </c>
     </row>
     <row r="86">
       <c r="A86" t="str">
@@ -1861,9 +1606,6 @@
       <c r="D86" t="str">
         <v>JP</v>
       </c>
-      <c r="E86" t="str">
-        <v/>
-      </c>
     </row>
     <row r="87">
       <c r="A87" t="str">
@@ -1878,9 +1620,6 @@
       <c r="D87" t="str">
         <v>JP</v>
       </c>
-      <c r="E87" t="str">
-        <v/>
-      </c>
     </row>
     <row r="88">
       <c r="A88" t="str">
@@ -1895,9 +1634,6 @@
       <c r="D88" t="str">
         <v>JP</v>
       </c>
-      <c r="E88" t="str">
-        <v/>
-      </c>
     </row>
     <row r="89">
       <c r="A89" t="str">
@@ -1912,9 +1648,6 @@
       <c r="D89" t="str">
         <v>JP</v>
       </c>
-      <c r="E89" t="str">
-        <v/>
-      </c>
     </row>
     <row r="90">
       <c r="A90" t="str">
@@ -1929,9 +1662,6 @@
       <c r="D90" t="str">
         <v>JP</v>
       </c>
-      <c r="E90" t="str">
-        <v/>
-      </c>
     </row>
     <row r="91">
       <c r="A91" t="str">
@@ -1946,9 +1676,6 @@
       <c r="D91" t="str">
         <v>JP</v>
       </c>
-      <c r="E91" t="str">
-        <v/>
-      </c>
     </row>
     <row r="92">
       <c r="A92" t="str">
@@ -1963,9 +1690,6 @@
       <c r="D92" t="str">
         <v>JP</v>
       </c>
-      <c r="E92" t="str">
-        <v/>
-      </c>
     </row>
     <row r="93">
       <c r="A93" t="str">
@@ -1980,9 +1704,6 @@
       <c r="D93" t="str">
         <v>JP</v>
       </c>
-      <c r="E93" t="str">
-        <v/>
-      </c>
     </row>
     <row r="94">
       <c r="A94" t="str">
@@ -1997,9 +1718,6 @@
       <c r="D94" t="str">
         <v>JP</v>
       </c>
-      <c r="E94" t="str">
-        <v/>
-      </c>
     </row>
     <row r="95">
       <c r="A95" t="str">
@@ -2014,9 +1732,6 @@
       <c r="D95" t="str">
         <v>JP</v>
       </c>
-      <c r="E95" t="str">
-        <v/>
-      </c>
     </row>
     <row r="96">
       <c r="A96" t="str">
@@ -2031,9 +1746,6 @@
       <c r="D96" t="str">
         <v>JP</v>
       </c>
-      <c r="E96" t="str">
-        <v/>
-      </c>
     </row>
     <row r="97">
       <c r="A97" t="str">
@@ -2048,9 +1760,6 @@
       <c r="D97" t="str">
         <v>FR</v>
       </c>
-      <c r="E97" t="str">
-        <v/>
-      </c>
     </row>
     <row r="98">
       <c r="A98" t="str">
@@ -2065,14 +1774,11 @@
       <c r="D98" t="str">
         <v>FR</v>
       </c>
-      <c r="E98" t="str">
-        <v/>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E98"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D98"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
updateXlsxWithCardsUrl.js -> update script structure
</commit_message>
<xml_diff>
--- a/excelPriceCards/cartes.xlsx
+++ b/excelPriceCards/cartes.xlsx
@@ -5,6 +5,9 @@
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
     <sheet name="28_01_2024" sheetId="2" r:id="rId2"/>
+    <sheet name="29_01_2024" sheetId="3" r:id="rId3"/>
+    <sheet name="30_01_2024" sheetId="4" r:id="rId4"/>
+    <sheet name="03_02_2024" sheetId="5" r:id="rId5"/>
   </sheets>
 </workbook>
 </file>
@@ -1785,6 +1788,1396 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E98"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Nom</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Numéro</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Série</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Langue</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Prix moyen</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>Noctali</v>
+      </c>
+      <c r="B2" t="str">
+        <v>85/69</v>
+      </c>
+      <c r="C2" t="str">
+        <v>S6A</v>
+      </c>
+      <c r="D2" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Givrali</v>
+      </c>
+      <c r="B3" t="str">
+        <v>25/69</v>
+      </c>
+      <c r="C3" t="str">
+        <v>S6A</v>
+      </c>
+      <c r="D3" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Nymphali</v>
+      </c>
+      <c r="B4" t="str">
+        <v>41/69</v>
+      </c>
+      <c r="C4" t="str">
+        <v>S6A</v>
+      </c>
+      <c r="D4" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Nocatli</v>
+      </c>
+      <c r="B5" t="str">
+        <v>48/69</v>
+      </c>
+      <c r="C5" t="str">
+        <v>S6A</v>
+      </c>
+      <c r="D5" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>Nymphali</v>
+      </c>
+      <c r="B6" t="str">
+        <v>40/69</v>
+      </c>
+      <c r="C6" t="str">
+        <v>S6A</v>
+      </c>
+      <c r="D6" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>Givrali</v>
+      </c>
+      <c r="B7" t="str">
+        <v>24/69</v>
+      </c>
+      <c r="C7" t="str">
+        <v>S6A</v>
+      </c>
+      <c r="D7" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>Aquali</v>
+      </c>
+      <c r="B8" t="str">
+        <v>15/69</v>
+      </c>
+      <c r="C8" t="str">
+        <v>S6A</v>
+      </c>
+      <c r="D8" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>Phyllali</v>
+      </c>
+      <c r="B9" t="str">
+        <v>002/69</v>
+      </c>
+      <c r="C9" t="str">
+        <v>S6A</v>
+      </c>
+      <c r="D9" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>Desseliande</v>
+      </c>
+      <c r="B10" t="str">
+        <v>68/67</v>
+      </c>
+      <c r="C10" t="str">
+        <v>S7R</v>
+      </c>
+      <c r="D10" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>Léviator</v>
+      </c>
+      <c r="B11" t="str">
+        <v>21/67</v>
+      </c>
+      <c r="C11" t="str">
+        <v>S7R</v>
+      </c>
+      <c r="D11" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>Rayquaza</v>
+      </c>
+      <c r="B12" t="str">
+        <v>47/67</v>
+      </c>
+      <c r="C12" t="str">
+        <v>S7R</v>
+      </c>
+      <c r="D12" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v xml:space="preserve">Leviator </v>
+      </c>
+      <c r="B13" t="str">
+        <v>20/67</v>
+      </c>
+      <c r="C13" t="str">
+        <v>S7R</v>
+      </c>
+      <c r="D13" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>Rayquaza</v>
+      </c>
+      <c r="B14" t="str">
+        <v>46/67</v>
+      </c>
+      <c r="C14" t="str">
+        <v>S7R</v>
+      </c>
+      <c r="D14" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>Pyrax</v>
+      </c>
+      <c r="B15" t="str">
+        <v>15/67</v>
+      </c>
+      <c r="C15" t="str">
+        <v>S7R</v>
+      </c>
+      <c r="D15" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>Desseliande</v>
+      </c>
+      <c r="B16" t="str">
+        <v>007/67</v>
+      </c>
+      <c r="C16" t="str">
+        <v>S7R</v>
+      </c>
+      <c r="D16" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>Dracolosse</v>
+      </c>
+      <c r="B17" t="str">
+        <v>42/67</v>
+      </c>
+      <c r="C17" t="str">
+        <v>S7R</v>
+      </c>
+      <c r="D17" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>Vmax Duralugon</v>
+      </c>
+      <c r="B18" t="str">
+        <v>285/184</v>
+      </c>
+      <c r="C18" t="str">
+        <v>S8B</v>
+      </c>
+      <c r="D18" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>V Scolocendre</v>
+      </c>
+      <c r="B19" t="str">
+        <v>22/184</v>
+      </c>
+      <c r="C19" t="str">
+        <v>S8B</v>
+      </c>
+      <c r="D19" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>V Noctali</v>
+      </c>
+      <c r="B20" t="str">
+        <v>100/184</v>
+      </c>
+      <c r="C20" t="str">
+        <v>S8B</v>
+      </c>
+      <c r="D20" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>V Zeraora</v>
+      </c>
+      <c r="B21" t="str">
+        <v>54/184</v>
+      </c>
+      <c r="C21" t="str">
+        <v>S8B</v>
+      </c>
+      <c r="D21" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>V Sulfura</v>
+      </c>
+      <c r="B22" t="str">
+        <v>96/184</v>
+      </c>
+      <c r="C22" t="str">
+        <v>S8B</v>
+      </c>
+      <c r="D22" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v xml:space="preserve">V Duralugon </v>
+      </c>
+      <c r="B23" t="str">
+        <v>122/184</v>
+      </c>
+      <c r="C23" t="str">
+        <v>S8B</v>
+      </c>
+      <c r="D23" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>V Mimiqui</v>
+      </c>
+      <c r="B24" t="str">
+        <v>76/184</v>
+      </c>
+      <c r="C24" t="str">
+        <v>S8B</v>
+      </c>
+      <c r="D24" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>Vmax Rayquaza</v>
+      </c>
+      <c r="B25" t="str">
+        <v>120/184</v>
+      </c>
+      <c r="C25" t="str">
+        <v>S8B</v>
+      </c>
+      <c r="D25" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>Vmax Pikachu</v>
+      </c>
+      <c r="B26" t="str">
+        <v>46/184</v>
+      </c>
+      <c r="C26" t="str">
+        <v>S8B</v>
+      </c>
+      <c r="D26" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v xml:space="preserve">Vmax Sylveroy </v>
+      </c>
+      <c r="B27" t="str">
+        <v>44/184</v>
+      </c>
+      <c r="C27" t="str">
+        <v>S8B</v>
+      </c>
+      <c r="D27" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>Pyroli</v>
+      </c>
+      <c r="B28" t="str">
+        <v>188/184</v>
+      </c>
+      <c r="C28" t="str">
+        <v>S8B</v>
+      </c>
+      <c r="D28" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>Evoli</v>
+      </c>
+      <c r="B29" t="str">
+        <v>210/184</v>
+      </c>
+      <c r="C29" t="str">
+        <v>S8B</v>
+      </c>
+      <c r="D29" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>Hexadron</v>
+      </c>
+      <c r="B30" t="str">
+        <v>201/184</v>
+      </c>
+      <c r="C30" t="str">
+        <v>S8B</v>
+      </c>
+      <c r="D30" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>V Corvaillus</v>
+      </c>
+      <c r="B31" t="str">
+        <v>248/184</v>
+      </c>
+      <c r="C31" t="str">
+        <v>S8B</v>
+      </c>
+      <c r="D31" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>V Mackogneur</v>
+      </c>
+      <c r="B32" t="str">
+        <v>71/172</v>
+      </c>
+      <c r="C32" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D32" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>V Amovénus</v>
+      </c>
+      <c r="B33" t="str">
+        <v>68/172</v>
+      </c>
+      <c r="C33" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D33" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>V Cerbyllin</v>
+      </c>
+      <c r="B34" t="str">
+        <v>131/172</v>
+      </c>
+      <c r="C34" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D34" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>V Regigigas</v>
+      </c>
+      <c r="B35" t="str">
+        <v>124/172</v>
+      </c>
+      <c r="C35" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D35" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>V Mewtwo</v>
+      </c>
+      <c r="B36" t="str">
+        <v>50/172</v>
+      </c>
+      <c r="C36" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D36" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>Guérilande</v>
+      </c>
+      <c r="B37" t="str">
+        <v>187/172</v>
+      </c>
+      <c r="C37" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D37" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>Plumeline</v>
+      </c>
+      <c r="B38" t="str">
+        <v>176/172</v>
+      </c>
+      <c r="C38" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D38" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>Castorno</v>
+      </c>
+      <c r="B39" t="str">
+        <v>200/172</v>
+      </c>
+      <c r="C39" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D39" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>Energie elect</v>
+      </c>
+      <c r="B40" t="str">
+        <v>254/172</v>
+      </c>
+      <c r="C40" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D40" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>Vstar Dialga</v>
+      </c>
+      <c r="B41" t="str">
+        <v>101/172</v>
+      </c>
+      <c r="C41" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D41" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>Vstar Giratina</v>
+      </c>
+      <c r="B42" t="str">
+        <v>111/172</v>
+      </c>
+      <c r="C42" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D42" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>Vmax Mew</v>
+      </c>
+      <c r="B43" t="str">
+        <v>54/172</v>
+      </c>
+      <c r="C43" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D43" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>Vstar Regigigas</v>
+      </c>
+      <c r="B44" t="str">
+        <v>125/172</v>
+      </c>
+      <c r="C44" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D44" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>Vitalité de Flo</v>
+      </c>
+      <c r="B45" t="str">
+        <v>243/172</v>
+      </c>
+      <c r="C45" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D45" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v>V Zacian</v>
+      </c>
+      <c r="B46" t="str">
+        <v>225/172</v>
+      </c>
+      <c r="C46" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D46" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>Dracaufeu Radieux</v>
+      </c>
+      <c r="B47" t="str">
+        <v>015/172</v>
+      </c>
+      <c r="C47" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D47" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v>Entei V</v>
+      </c>
+      <c r="B48" t="str">
+        <v>213/172</v>
+      </c>
+      <c r="C48" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D48" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="str">
+        <v>Rayquaza VMAX</v>
+      </c>
+      <c r="B49" t="str">
+        <v>108/172</v>
+      </c>
+      <c r="C49" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D49" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="str">
+        <v>Palkia Originel VSTAR</v>
+      </c>
+      <c r="B50" t="str">
+        <v>028/172</v>
+      </c>
+      <c r="C50" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D50" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="str">
+        <v>Dialga Originel VSTAR</v>
+      </c>
+      <c r="B51" t="str">
+        <v>101/172</v>
+      </c>
+      <c r="C51" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D51" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="str">
+        <v>Roublenard</v>
+      </c>
+      <c r="B52" t="str">
+        <v>192/172</v>
+      </c>
+      <c r="C52" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D52" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="str">
+        <v>Salarsen</v>
+      </c>
+      <c r="B53" t="str">
+        <v>181/172</v>
+      </c>
+      <c r="C53" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D53" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="str">
+        <v>Ecrémeuf</v>
+      </c>
+      <c r="B54" t="str">
+        <v>199/172</v>
+      </c>
+      <c r="C54" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D54" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="str">
+        <v>Zoroark de Hisui V</v>
+      </c>
+      <c r="B55" t="str">
+        <v>128/172</v>
+      </c>
+      <c r="C55" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D55" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="str">
+        <v>Zeraora V</v>
+      </c>
+      <c r="B56" t="str">
+        <v>040/172</v>
+      </c>
+      <c r="C56" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D56" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="str">
+        <v>Giratina V</v>
+      </c>
+      <c r="B57" t="str">
+        <v>110/172</v>
+      </c>
+      <c r="C57" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D57" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="str">
+        <v>Sorcilence</v>
+      </c>
+      <c r="B58" t="str">
+        <v>065/172</v>
+      </c>
+      <c r="C58" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D58" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="str">
+        <v>Carchacrock V</v>
+      </c>
+      <c r="B59" t="str">
+        <v>109/172</v>
+      </c>
+      <c r="C59" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D59" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="str">
+        <v>Recherche Professorale</v>
+      </c>
+      <c r="B60" t="str">
+        <v>248/172</v>
+      </c>
+      <c r="C60" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D60" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="str">
+        <v>Energie Psy</v>
+      </c>
+      <c r="B61" t="str">
+        <v>255/172</v>
+      </c>
+      <c r="C61" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D61" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="str">
+        <v>Brutalibré Radieux</v>
+      </c>
+      <c r="B62" t="str">
+        <v>078/172</v>
+      </c>
+      <c r="C62" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D62" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="str">
+        <v>Giratina Holo</v>
+      </c>
+      <c r="B63" t="str">
+        <v>10/127</v>
+      </c>
+      <c r="C63" t="str">
+        <v>Platine</v>
+      </c>
+      <c r="D63" t="str">
+        <v>FR</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="str">
+        <v>Giratina VSTAR</v>
+      </c>
+      <c r="B64" t="str">
+        <v>261/172</v>
+      </c>
+      <c r="C64" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D64" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="str">
+        <v>Energie Tênebre</v>
+      </c>
+      <c r="B65" t="str">
+        <v>257/172</v>
+      </c>
+      <c r="C65" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D65" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="str">
+        <v>Energie Acier</v>
+      </c>
+      <c r="B66" t="str">
+        <v>258/172</v>
+      </c>
+      <c r="C66" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D66" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="str">
+        <v>Energie Feu</v>
+      </c>
+      <c r="B67" t="str">
+        <v>252/172</v>
+      </c>
+      <c r="C67" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D67" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="str">
+        <v>Regigigas VSTAR</v>
+      </c>
+      <c r="B68" t="str">
+        <v>233/172</v>
+      </c>
+      <c r="C68" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D68" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="str">
+        <v>Entei V</v>
+      </c>
+      <c r="B69" t="str">
+        <v>213/172</v>
+      </c>
+      <c r="C69" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D69" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="str">
+        <v xml:space="preserve">Suicune </v>
+      </c>
+      <c r="B70" t="str">
+        <v>215/172</v>
+      </c>
+      <c r="C70" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D70" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="str">
+        <v>Clamiral</v>
+      </c>
+      <c r="B71" t="str">
+        <v>229/172</v>
+      </c>
+      <c r="C71" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D71" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="str">
+        <v>Darkrai VSTAR</v>
+      </c>
+      <c r="B72" t="str">
+        <v>228/172</v>
+      </c>
+      <c r="C72" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D72" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="str">
+        <v>Deoxy Vmax</v>
+      </c>
+      <c r="B73" t="str">
+        <v>222/172</v>
+      </c>
+      <c r="C73" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D73" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="str">
+        <v>Zacian V</v>
+      </c>
+      <c r="B74" t="str">
+        <v>225/172</v>
+      </c>
+      <c r="C74" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D74" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="str">
+        <v>Hoopa</v>
+      </c>
+      <c r="B75" t="str">
+        <v>231/172</v>
+      </c>
+      <c r="C75" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D75" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="str">
+        <v>Clamiral Vstar</v>
+      </c>
+      <c r="B76" t="str">
+        <v>230/172</v>
+      </c>
+      <c r="C76" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D76" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="str">
+        <v>Raikou</v>
+      </c>
+      <c r="B77" t="str">
+        <v>218/172</v>
+      </c>
+      <c r="C77" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D77" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="str">
+        <v>Drascore</v>
+      </c>
+      <c r="B78" t="str">
+        <v>227/172</v>
+      </c>
+      <c r="C78" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D78" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="str">
+        <v>Keldeo</v>
+      </c>
+      <c r="B79" t="str">
+        <v>179/172</v>
+      </c>
+      <c r="C79" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D79" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="str">
+        <v>Insolourdo</v>
+      </c>
+      <c r="B80" t="str">
+        <v>198/172</v>
+      </c>
+      <c r="C80" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D80" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="str">
+        <v>Maganon</v>
+      </c>
+      <c r="B81" t="str">
+        <v>175/172</v>
+      </c>
+      <c r="C81" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D81" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="str">
+        <v>Locklass</v>
+      </c>
+      <c r="B82" t="str">
+        <v>177/172</v>
+      </c>
+      <c r="C82" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D82" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="str">
+        <v>Elekable</v>
+      </c>
+      <c r="B83" t="str">
+        <v>180/172</v>
+      </c>
+      <c r="C83" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D83" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="str">
+        <v>Séléroc</v>
+      </c>
+      <c r="B84" t="str">
+        <v>184/172</v>
+      </c>
+      <c r="C84" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D84" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="str">
+        <v>Electhor de Galar</v>
+      </c>
+      <c r="B85" t="str">
+        <v>188/172</v>
+      </c>
+      <c r="C85" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D85" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="str">
+        <v>Absol</v>
+      </c>
+      <c r="B86" t="str">
+        <v>191/172</v>
+      </c>
+      <c r="C86" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D86" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="str">
+        <v>Roublenard</v>
+      </c>
+      <c r="B87" t="str">
+        <v>192/172</v>
+      </c>
+      <c r="C87" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D87" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="str">
+        <v>Magnézone</v>
+      </c>
+      <c r="B88" t="str">
+        <v>193/172</v>
+      </c>
+      <c r="C88" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D88" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="str">
+        <v>Voltorbe de Hisui</v>
+      </c>
+      <c r="B89" t="str">
+        <v>173/172</v>
+      </c>
+      <c r="C89" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D89" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="str">
+        <v>Altaria</v>
+      </c>
+      <c r="B90" t="str">
+        <v>194/172</v>
+      </c>
+      <c r="C90" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D90" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="str">
+        <v>Mew</v>
+      </c>
+      <c r="B91" t="str">
+        <v>183/172</v>
+      </c>
+      <c r="C91" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D91" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="str">
+        <v>Melokrik</v>
+      </c>
+      <c r="B92" t="str">
+        <v>174/172</v>
+      </c>
+      <c r="C92" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D92" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="str">
+        <v>Diancy</v>
+      </c>
+      <c r="B93" t="str">
+        <v>186/172</v>
+      </c>
+      <c r="C93" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D93" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="str">
+        <v>Sulfura Galar</v>
+      </c>
+      <c r="B94" t="str">
+        <v>190/172</v>
+      </c>
+      <c r="C94" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D94" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="str">
+        <v>Muplodocus</v>
+      </c>
+      <c r="B95" t="str">
+        <v>196/172</v>
+      </c>
+      <c r="C95" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D95" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="str">
+        <v>Artikodin Galar</v>
+      </c>
+      <c r="B96" t="str">
+        <v>182/172</v>
+      </c>
+      <c r="C96" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D96" t="str">
+        <v>JP</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="str">
+        <v>Tortank Ex</v>
+      </c>
+      <c r="B97" t="str">
+        <v>200/165</v>
+      </c>
+      <c r="C97">
+        <v>151</v>
+      </c>
+      <c r="D97" t="str">
+        <v>FR</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="str">
+        <v>Charisme de Giovanni</v>
+      </c>
+      <c r="B98" t="str">
+        <v>204/165</v>
+      </c>
+      <c r="C98">
+        <v>151</v>
+      </c>
+      <c r="D98" t="str">
+        <v>FR</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:E98"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F98"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
@@ -3465,4 +4858,3372 @@
     <ignoredError numberStoredAsText="1" sqref="A1:F98"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F98"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Nom</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Numéro</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Série</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Langue</v>
+      </c>
+      <c r="E1" t="str">
+        <v/>
+      </c>
+      <c r="F1" t="str">
+        <v>Prix moyen</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>Noctali</v>
+      </c>
+      <c r="B2" t="str">
+        <v>85/69</v>
+      </c>
+      <c r="C2" t="str">
+        <v>S6A</v>
+      </c>
+      <c r="D2" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E2" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Eevee-Heroes/Umbreon-V-V3-s6a085?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Givrali</v>
+      </c>
+      <c r="B3" t="str">
+        <v>25/69</v>
+      </c>
+      <c r="C3" t="str">
+        <v>S6A</v>
+      </c>
+      <c r="D3" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E3" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Eevee-Heroes/Glaceon-VMAX-V1?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Nymphali</v>
+      </c>
+      <c r="B4" t="str">
+        <v>41/69</v>
+      </c>
+      <c r="C4" t="str">
+        <v>S6A</v>
+      </c>
+      <c r="D4" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E4" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Eevee-Heroes/Sylveon-VMAX-V1-s6a041?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Nocatli</v>
+      </c>
+      <c r="B5" t="str">
+        <v>48/69</v>
+      </c>
+      <c r="C5" t="str">
+        <v>S6A</v>
+      </c>
+      <c r="D5" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E5" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Eevee-Heroes/Umbreon-VMAX-V1?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>Nymphali</v>
+      </c>
+      <c r="B6" t="str">
+        <v>40/69</v>
+      </c>
+      <c r="C6" t="str">
+        <v>S6A</v>
+      </c>
+      <c r="D6" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E6" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Eevee-Heroes/Sylveon-V-V1?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>Givrali</v>
+      </c>
+      <c r="B7" t="str">
+        <v>24/69</v>
+      </c>
+      <c r="C7" t="str">
+        <v>S6A</v>
+      </c>
+      <c r="D7" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E7" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Eevee-Heroes/Glaceon-V-V1-s6a024?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>Aquali</v>
+      </c>
+      <c r="B8" t="str">
+        <v>15/69</v>
+      </c>
+      <c r="C8" t="str">
+        <v>S6A</v>
+      </c>
+      <c r="D8" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E8" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Eevee-Heroes/Vaporeon-V-V1?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>Phyllali</v>
+      </c>
+      <c r="B9" t="str">
+        <v>002/69</v>
+      </c>
+      <c r="C9" t="str">
+        <v>S6A</v>
+      </c>
+      <c r="D9" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E9" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Eevee-Heroes/Leafeon-V-V1?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>Desseliande</v>
+      </c>
+      <c r="B10" t="str">
+        <v>68/67</v>
+      </c>
+      <c r="C10" t="str">
+        <v>S7R</v>
+      </c>
+      <c r="D10" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E10" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Blue-Sky-Stream/Trevenant-V-V2?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>Léviator</v>
+      </c>
+      <c r="B11" t="str">
+        <v>21/67</v>
+      </c>
+      <c r="C11" t="str">
+        <v>S7R</v>
+      </c>
+      <c r="D11" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E11" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Blue-Sky-Stream/Gyarados-VMAX-V1?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>Rayquaza</v>
+      </c>
+      <c r="B12" t="str">
+        <v>47/67</v>
+      </c>
+      <c r="C12" t="str">
+        <v>S7R</v>
+      </c>
+      <c r="D12" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E12" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Blue-Sky-Stream/Rayquaza-VMAX-V1-s7R047?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v xml:space="preserve">Leviator </v>
+      </c>
+      <c r="B13" t="str">
+        <v>20/67</v>
+      </c>
+      <c r="C13" t="str">
+        <v>S7R</v>
+      </c>
+      <c r="D13" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E13" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Blue-Sky-Stream/Gyarados-V-V1-s7R020?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>Rayquaza</v>
+      </c>
+      <c r="B14" t="str">
+        <v>46/67</v>
+      </c>
+      <c r="C14" t="str">
+        <v>S7R</v>
+      </c>
+      <c r="D14" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E14" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Blue-Sky-Stream/Rayquaza-V-V1?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>Pyrax</v>
+      </c>
+      <c r="B15" t="str">
+        <v>15/67</v>
+      </c>
+      <c r="C15" t="str">
+        <v>S7R</v>
+      </c>
+      <c r="D15" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E15" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Blue-Sky-Stream/Volcarona-V-V1-s7R015?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>Desseliande</v>
+      </c>
+      <c r="B16" t="str">
+        <v>007/67</v>
+      </c>
+      <c r="C16" t="str">
+        <v>S7R</v>
+      </c>
+      <c r="D16" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E16" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Blue-Sky-Stream/Trevenant-V-V1?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>Dracolosse</v>
+      </c>
+      <c r="B17" t="str">
+        <v>42/67</v>
+      </c>
+      <c r="C17" t="str">
+        <v>S7R</v>
+      </c>
+      <c r="D17" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E17" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Blue-Sky-Stream/Dragonite-V-V1?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>Vmax Duralugon</v>
+      </c>
+      <c r="B18" t="str">
+        <v>285/184</v>
+      </c>
+      <c r="C18" t="str">
+        <v>S8B</v>
+      </c>
+      <c r="D18" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E18" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VMAX-Climax/Duraludon-VMAX-V3-s8b285?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>V Scolocendre</v>
+      </c>
+      <c r="B19" t="str">
+        <v>22/184</v>
+      </c>
+      <c r="C19" t="str">
+        <v>S8B</v>
+      </c>
+      <c r="D19" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E19" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VMAX-Climax/Centiskorch-V-V1-s8b022?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>V Noctali</v>
+      </c>
+      <c r="B20" t="str">
+        <v>100/184</v>
+      </c>
+      <c r="C20" t="str">
+        <v>S8B</v>
+      </c>
+      <c r="D20" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E20" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VMAX-Climax/Umbreon-V-V1-s8b100?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>V Zeraora</v>
+      </c>
+      <c r="B21" t="str">
+        <v>54/184</v>
+      </c>
+      <c r="C21" t="str">
+        <v>S8B</v>
+      </c>
+      <c r="D21" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E21" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VMAX-Climax/Zeraora-V-V1-s8b054?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>V Sulfura</v>
+      </c>
+      <c r="B22" t="str">
+        <v>96/184</v>
+      </c>
+      <c r="C22" t="str">
+        <v>S8B</v>
+      </c>
+      <c r="D22" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E22" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VMAX-Climax/Galarian-Moltres-V-V1-s8b096?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v xml:space="preserve">V Duralugon </v>
+      </c>
+      <c r="B23" t="str">
+        <v>122/184</v>
+      </c>
+      <c r="C23" t="str">
+        <v>S8B</v>
+      </c>
+      <c r="D23" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E23" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VMAX-Climax/Duraludon-V?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>V Mimiqui</v>
+      </c>
+      <c r="B24" t="str">
+        <v>76/184</v>
+      </c>
+      <c r="C24" t="str">
+        <v>S8B</v>
+      </c>
+      <c r="D24" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E24" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VMAX-Climax/Mimikyu-V-V1-s8b076?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>Vmax Rayquaza</v>
+      </c>
+      <c r="B25" t="str">
+        <v>120/184</v>
+      </c>
+      <c r="C25" t="str">
+        <v>S8B</v>
+      </c>
+      <c r="D25" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E25" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VMAX-Climax/Rayquaza-VMAX-V1-s8b120?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>Vmax Pikachu</v>
+      </c>
+      <c r="B26" t="str">
+        <v>46/184</v>
+      </c>
+      <c r="C26" t="str">
+        <v>S8B</v>
+      </c>
+      <c r="D26" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E26" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VMAX-Climax/Pikachu-VMAX-V1-s8b046?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v xml:space="preserve">Vmax Sylveroy </v>
+      </c>
+      <c r="B27" t="str">
+        <v>44/184</v>
+      </c>
+      <c r="C27" t="str">
+        <v>S8B</v>
+      </c>
+      <c r="D27" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E27" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VMAX-Climax/Ice-Rider-Calyrex-VMAX-V1-s8b044?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>Pyroli</v>
+      </c>
+      <c r="B28" t="str">
+        <v>188/184</v>
+      </c>
+      <c r="C28" t="str">
+        <v>S8B</v>
+      </c>
+      <c r="D28" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E28" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VMAX-Climax/Flareon-V2-s8b188?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>Evoli</v>
+      </c>
+      <c r="B29" t="str">
+        <v>210/184</v>
+      </c>
+      <c r="C29" t="str">
+        <v>S8B</v>
+      </c>
+      <c r="D29" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E29" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VMAX-Climax/Eevee-V2-s8b210?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>Hexadron</v>
+      </c>
+      <c r="B30" t="str">
+        <v>201/184</v>
+      </c>
+      <c r="C30" t="str">
+        <v>S8B</v>
+      </c>
+      <c r="D30" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E30" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VMAX-Climax/Falinks-V1-s8b089?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>V Corvaillus</v>
+      </c>
+      <c r="B31" t="str">
+        <v>248/184</v>
+      </c>
+      <c r="C31" t="str">
+        <v>S8B</v>
+      </c>
+      <c r="D31" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E31" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VMAX-Climax/Corviknight-V-V2-s8b248?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>V Mackogneur</v>
+      </c>
+      <c r="B32" t="str">
+        <v>71/172</v>
+      </c>
+      <c r="C32" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D32" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E32" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Machamp-V-s12a071?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>V Amovénus</v>
+      </c>
+      <c r="B33" t="str">
+        <v>68/172</v>
+      </c>
+      <c r="C33" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D33" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E33" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Enamorus-V-s12a068?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>V Cerbyllin</v>
+      </c>
+      <c r="B34" t="str">
+        <v>131/172</v>
+      </c>
+      <c r="C34" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D34" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E34" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Wyrdeer-V-s12a131?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>V Regigigas</v>
+      </c>
+      <c r="B35" t="str">
+        <v>124/172</v>
+      </c>
+      <c r="C35" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D35" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E35" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Regigigas-V-s12a124?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>V Mewtwo</v>
+      </c>
+      <c r="B36" t="str">
+        <v>50/172</v>
+      </c>
+      <c r="C36" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D36" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E36" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Mewtwo-V-s12a050?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>Guérilande</v>
+      </c>
+      <c r="B37" t="str">
+        <v>187/172</v>
+      </c>
+      <c r="C37" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D37" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E37" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Comfey-V2-s12a187?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>Plumeline</v>
+      </c>
+      <c r="B38" t="str">
+        <v>176/172</v>
+      </c>
+      <c r="C38" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D38" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E38" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Oricorio-V2-s12a176?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>Castorno</v>
+      </c>
+      <c r="B39" t="str">
+        <v>200/172</v>
+      </c>
+      <c r="C39" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D39" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E39" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Bibarel-V2-s12a200?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>Energie elect</v>
+      </c>
+      <c r="B40" t="str">
+        <v>254/172</v>
+      </c>
+      <c r="C40" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D40" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E40" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Lightning-Energy-s12a254?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>Vstar Dialga</v>
+      </c>
+      <c r="B41" t="str">
+        <v>101/172</v>
+      </c>
+      <c r="C41" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D41" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E41" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Origin-Forme-Dialga-VSTAR-V1-s12a101?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>Vstar Giratina</v>
+      </c>
+      <c r="B42" t="str">
+        <v>111/172</v>
+      </c>
+      <c r="C42" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D42" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E42" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Giratina-VSTAR-V1-s12a111?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>Vmax Mew</v>
+      </c>
+      <c r="B43" t="str">
+        <v>54/172</v>
+      </c>
+      <c r="C43" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D43" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E43" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Mew-VMAX-s12a054?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>Vstar Regigigas</v>
+      </c>
+      <c r="B44" t="str">
+        <v>125/172</v>
+      </c>
+      <c r="C44" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D44" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E44" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Regigigas-VSTAR-V1-s12a125?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>Vitalité de Flo</v>
+      </c>
+      <c r="B45" t="str">
+        <v>243/172</v>
+      </c>
+      <c r="C45" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D45" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E45" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Gardenias-Vigor-V2-s12a243?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v>V Zacian</v>
+      </c>
+      <c r="B46" t="str">
+        <v>225/172</v>
+      </c>
+      <c r="C46" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D46" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E46" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Zacian-V-V2-s12a225?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>Dracaufeu Radieux</v>
+      </c>
+      <c r="B47" t="str">
+        <v>015/172</v>
+      </c>
+      <c r="C47" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D47" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E47" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Radiant-Charizard-s12a015?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v>Entei V</v>
+      </c>
+      <c r="B48" t="str">
+        <v>213/172</v>
+      </c>
+      <c r="C48" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D48" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E48" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Entei-V-V2-s12a213?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="str">
+        <v>Rayquaza VMAX</v>
+      </c>
+      <c r="B49" t="str">
+        <v>108/172</v>
+      </c>
+      <c r="C49" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D49" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E49" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Rayquaza-VMAX-s12a108?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="str">
+        <v>Palkia Originel VSTAR</v>
+      </c>
+      <c r="B50" t="str">
+        <v>028/172</v>
+      </c>
+      <c r="C50" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D50" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E50" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Origin-Forme-Palkia-VSTAR-V1-s12a028?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="str">
+        <v>Dialga Originel VSTAR</v>
+      </c>
+      <c r="B51" t="str">
+        <v>101/172</v>
+      </c>
+      <c r="C51" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D51" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E51" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Origin-Forme-Dialga-VSTAR-V1-s12a101?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="str">
+        <v>Roublenard</v>
+      </c>
+      <c r="B52" t="str">
+        <v>192/172</v>
+      </c>
+      <c r="C52" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D52" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E52" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Thievul-V2-s12a192?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="str">
+        <v>Salarsen</v>
+      </c>
+      <c r="B53" t="str">
+        <v>181/172</v>
+      </c>
+      <c r="C53" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D53" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E53" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Toxtricity-V2-s12a181?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="str">
+        <v>Ecrémeuf</v>
+      </c>
+      <c r="B54" t="str">
+        <v>199/172</v>
+      </c>
+      <c r="C54" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D54" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E54" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Miltank-V2-s12a199?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="str">
+        <v>Zoroark de Hisui V</v>
+      </c>
+      <c r="B55" t="str">
+        <v>128/172</v>
+      </c>
+      <c r="C55" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D55" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E55" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Hisuian-Zoroark-V-s12a128?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="str">
+        <v>Zeraora V</v>
+      </c>
+      <c r="B56" t="str">
+        <v>040/172</v>
+      </c>
+      <c r="C56" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D56" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E56" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Zeraora-V-s12a040?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="str">
+        <v>Giratina V</v>
+      </c>
+      <c r="B57" t="str">
+        <v>110/172</v>
+      </c>
+      <c r="C57" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D57" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E57" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Giratina-V-s12a110?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="str">
+        <v>Sorcilence</v>
+      </c>
+      <c r="B58" t="str">
+        <v>065/172</v>
+      </c>
+      <c r="C58" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D58" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E58" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Hatterene-V-s12a065?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="str">
+        <v>Carchacrock V</v>
+      </c>
+      <c r="B59" t="str">
+        <v>109/172</v>
+      </c>
+      <c r="C59" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D59" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E59" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Garchomp-V-s12a109?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="str">
+        <v>Recherche Professorale</v>
+      </c>
+      <c r="B60" t="str">
+        <v>248/172</v>
+      </c>
+      <c r="C60" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D60" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E60" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Professors-Research-V2-s12a248?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="str">
+        <v>Energie Psy</v>
+      </c>
+      <c r="B61" t="str">
+        <v>255/172</v>
+      </c>
+      <c r="C61" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D61" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E61" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Psychic-Energy-s12a255?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="str">
+        <v>Brutalibré Radieux</v>
+      </c>
+      <c r="B62" t="str">
+        <v>078/172</v>
+      </c>
+      <c r="C62" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D62" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E62" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Radiant-Hawlucha-s12a078?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="str">
+        <v>Giratina Holo</v>
+      </c>
+      <c r="B63" t="str">
+        <v>10/127</v>
+      </c>
+      <c r="C63" t="str">
+        <v>Platine</v>
+      </c>
+      <c r="D63" t="str">
+        <v>FR</v>
+      </c>
+      <c r="E63" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Platinum/Giratina-Lv63-PL10?language=2&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="str">
+        <v>Giratina VSTAR</v>
+      </c>
+      <c r="B64" t="str">
+        <v>261/172</v>
+      </c>
+      <c r="C64" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D64" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E64" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Giratina-VSTAR-V2-s12a261?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="str">
+        <v>Energie Tênebre</v>
+      </c>
+      <c r="B65" t="str">
+        <v>257/172</v>
+      </c>
+      <c r="C65" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D65" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E65" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Darkness-Energy-s12a257?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="str">
+        <v>Energie Acier</v>
+      </c>
+      <c r="B66" t="str">
+        <v>258/172</v>
+      </c>
+      <c r="C66" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D66" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E66" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Metal-Energy-s12a258?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="str">
+        <v>Energie Feu</v>
+      </c>
+      <c r="B67" t="str">
+        <v>252/172</v>
+      </c>
+      <c r="C67" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D67" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E67" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Fire-Energy-s12a252?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="str">
+        <v>Regigigas VSTAR</v>
+      </c>
+      <c r="B68" t="str">
+        <v>233/172</v>
+      </c>
+      <c r="C68" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D68" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E68" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Regigigas-VSTAR-V2-s12a233?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="str">
+        <v>Entei V</v>
+      </c>
+      <c r="B69" t="str">
+        <v>213/172</v>
+      </c>
+      <c r="C69" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D69" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E69" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Entei-V-V2-s12a213?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="str">
+        <v xml:space="preserve">Suicune </v>
+      </c>
+      <c r="B70" t="str">
+        <v>215/172</v>
+      </c>
+      <c r="C70" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D70" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E70" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Suicune-V-V2-s12a215?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="str">
+        <v>Clamiral</v>
+      </c>
+      <c r="B71" t="str">
+        <v>229/172</v>
+      </c>
+      <c r="C71" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D71" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E71" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Hisuian-Samurott-V-V2-s12a229?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="str">
+        <v>Darkrai VSTAR</v>
+      </c>
+      <c r="B72" t="str">
+        <v>228/172</v>
+      </c>
+      <c r="C72" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D72" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E72" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Darkrai-VSTAR-s12a228?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="str">
+        <v>Deoxy Vmax</v>
+      </c>
+      <c r="B73" t="str">
+        <v>222/172</v>
+      </c>
+      <c r="C73" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D73" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E73" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Deoxys-VMAX-s12a222?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="str">
+        <v>Zacian V</v>
+      </c>
+      <c r="B74" t="str">
+        <v>225/172</v>
+      </c>
+      <c r="C74" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D74" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E74" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Zacian-V-V2-s12a225?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="str">
+        <v>Hoopa</v>
+      </c>
+      <c r="B75" t="str">
+        <v>231/172</v>
+      </c>
+      <c r="C75" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D75" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E75" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Hoopa-V-s12a231?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="str">
+        <v>Clamiral Vstar</v>
+      </c>
+      <c r="B76" t="str">
+        <v>230/172</v>
+      </c>
+      <c r="C76" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D76" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E76" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Hisuian-Samurott-VSTAR-V2-s12a230?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="str">
+        <v>Raikou</v>
+      </c>
+      <c r="B77" t="str">
+        <v>218/172</v>
+      </c>
+      <c r="C77" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D77" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E77" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Raikou-V-V2-s12a218?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="str">
+        <v>Drascore</v>
+      </c>
+      <c r="B78" t="str">
+        <v>227/172</v>
+      </c>
+      <c r="C78" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D78" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E78" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Drapion-V-V2-s12a227?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="str">
+        <v>Keldeo</v>
+      </c>
+      <c r="B79" t="str">
+        <v>179/172</v>
+      </c>
+      <c r="C79" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D79" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E79" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Keldeo-V2-s12a179?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="str">
+        <v>Insolourdo</v>
+      </c>
+      <c r="B80" t="str">
+        <v>198/172</v>
+      </c>
+      <c r="C80" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D80" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E80" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Dunsparce-V2-s12a198?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="str">
+        <v>Maganon</v>
+      </c>
+      <c r="B81" t="str">
+        <v>175/172</v>
+      </c>
+      <c r="C81" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D81" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E81" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Magmortar-V2-s12a175?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="str">
+        <v>Locklass</v>
+      </c>
+      <c r="B82" t="str">
+        <v>177/172</v>
+      </c>
+      <c r="C82" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D82" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E82" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Lapras-V2-s12a177?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="str">
+        <v>Elekable</v>
+      </c>
+      <c r="B83" t="str">
+        <v>180/172</v>
+      </c>
+      <c r="C83" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D83" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E83" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Electivire-V2-s12a180?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="str">
+        <v>Séléroc</v>
+      </c>
+      <c r="B84" t="str">
+        <v>184/172</v>
+      </c>
+      <c r="C84" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D84" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E84" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Lunatone-V2-s12a184?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="str">
+        <v>Electhor de Galar</v>
+      </c>
+      <c r="B85" t="str">
+        <v>188/172</v>
+      </c>
+      <c r="C85" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D85" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E85" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Galarian-Zapdos-V2-s12a188?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="str">
+        <v>Absol</v>
+      </c>
+      <c r="B86" t="str">
+        <v>191/172</v>
+      </c>
+      <c r="C86" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D86" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E86" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Absol-V2-s12a191?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="str">
+        <v>Roublenard</v>
+      </c>
+      <c r="B87" t="str">
+        <v>192/172</v>
+      </c>
+      <c r="C87" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D87" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E87" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Thievul-V2-s12a192?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="str">
+        <v>Magnézone</v>
+      </c>
+      <c r="B88" t="str">
+        <v>193/172</v>
+      </c>
+      <c r="C88" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D88" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E88" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Magnezone-V2-s12a193?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="str">
+        <v>Voltorbe de Hisui</v>
+      </c>
+      <c r="B89" t="str">
+        <v>173/172</v>
+      </c>
+      <c r="C89" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D89" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E89" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Hisuian-Voltorb-V2-s12a173?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="str">
+        <v>Altaria</v>
+      </c>
+      <c r="B90" t="str">
+        <v>194/172</v>
+      </c>
+      <c r="C90" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D90" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E90" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Altaria-V2-s12a194?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="str">
+        <v>Mew</v>
+      </c>
+      <c r="B91" t="str">
+        <v>183/172</v>
+      </c>
+      <c r="C91" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D91" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E91" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Mew-V2-s12a183?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="str">
+        <v>Melokrik</v>
+      </c>
+      <c r="B92" t="str">
+        <v>174/172</v>
+      </c>
+      <c r="C92" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D92" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E92" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Kricketune-V2-s12a174?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="str">
+        <v>Diancy</v>
+      </c>
+      <c r="B93" t="str">
+        <v>186/172</v>
+      </c>
+      <c r="C93" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D93" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E93" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Diancie-V2-s12a186?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="str">
+        <v>Sulfura Galar</v>
+      </c>
+      <c r="B94" t="str">
+        <v>190/172</v>
+      </c>
+      <c r="C94" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D94" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E94" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Galarian-Moltres-V2-s12a190?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="str">
+        <v>Muplodocus</v>
+      </c>
+      <c r="B95" t="str">
+        <v>196/172</v>
+      </c>
+      <c r="C95" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D95" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E95" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Hisuian-Goodra-V2-s12a196?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="str">
+        <v>Artikodin Galar</v>
+      </c>
+      <c r="B96" t="str">
+        <v>182/172</v>
+      </c>
+      <c r="C96" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D96" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E96" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Galarian-Articuno-V2-s12a182?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="str">
+        <v>Tortank Ex</v>
+      </c>
+      <c r="B97" t="str">
+        <v>200/165</v>
+      </c>
+      <c r="C97">
+        <v>151</v>
+      </c>
+      <c r="D97" t="str">
+        <v>FR</v>
+      </c>
+      <c r="E97" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/151/Blastoise-ex-V3-MEW200?language=2&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="str">
+        <v>Charisme de Giovanni</v>
+      </c>
+      <c r="B98" t="str">
+        <v>204/165</v>
+      </c>
+      <c r="C98">
+        <v>151</v>
+      </c>
+      <c r="D98" t="str">
+        <v>FR</v>
+      </c>
+      <c r="E98" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/151/Giovannis-Charisma-V3-MEW204?language=2&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:F98"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F98"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Nom</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Numéro</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Série</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Langue</v>
+      </c>
+      <c r="E1" t="str">
+        <v/>
+      </c>
+      <c r="F1" t="str">
+        <v>Prix moyen</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>Noctali</v>
+      </c>
+      <c r="B2" t="str">
+        <v>85/69</v>
+      </c>
+      <c r="C2" t="str">
+        <v>S6A</v>
+      </c>
+      <c r="D2" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E2" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Eevee-Heroes/Umbreon-V-V3-s6a085?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Givrali</v>
+      </c>
+      <c r="B3" t="str">
+        <v>25/69</v>
+      </c>
+      <c r="C3" t="str">
+        <v>S6A</v>
+      </c>
+      <c r="D3" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E3" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Eevee-Heroes/Glaceon-VMAX-V1?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Nymphali</v>
+      </c>
+      <c r="B4" t="str">
+        <v>41/69</v>
+      </c>
+      <c r="C4" t="str">
+        <v>S6A</v>
+      </c>
+      <c r="D4" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E4" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Eevee-Heroes/Sylveon-VMAX-V1-s6a041?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Nocatli</v>
+      </c>
+      <c r="B5" t="str">
+        <v>48/69</v>
+      </c>
+      <c r="C5" t="str">
+        <v>S6A</v>
+      </c>
+      <c r="D5" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E5" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Eevee-Heroes/Umbreon-VMAX-V1?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>Nymphali</v>
+      </c>
+      <c r="B6" t="str">
+        <v>40/69</v>
+      </c>
+      <c r="C6" t="str">
+        <v>S6A</v>
+      </c>
+      <c r="D6" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E6" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Eevee-Heroes/Sylveon-V-V1?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>Givrali</v>
+      </c>
+      <c r="B7" t="str">
+        <v>24/69</v>
+      </c>
+      <c r="C7" t="str">
+        <v>S6A</v>
+      </c>
+      <c r="D7" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E7" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Eevee-Heroes/Glaceon-V-V1-s6a024?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>Aquali</v>
+      </c>
+      <c r="B8" t="str">
+        <v>15/69</v>
+      </c>
+      <c r="C8" t="str">
+        <v>S6A</v>
+      </c>
+      <c r="D8" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E8" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Eevee-Heroes/Vaporeon-V-V1?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>Phyllali</v>
+      </c>
+      <c r="B9" t="str">
+        <v>002/69</v>
+      </c>
+      <c r="C9" t="str">
+        <v>S6A</v>
+      </c>
+      <c r="D9" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E9" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Eevee-Heroes/Leafeon-V-V1?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>Desseliande</v>
+      </c>
+      <c r="B10" t="str">
+        <v>68/67</v>
+      </c>
+      <c r="C10" t="str">
+        <v>S7R</v>
+      </c>
+      <c r="D10" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E10" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Blue-Sky-Stream/Trevenant-V-V2?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>Léviator</v>
+      </c>
+      <c r="B11" t="str">
+        <v>21/67</v>
+      </c>
+      <c r="C11" t="str">
+        <v>S7R</v>
+      </c>
+      <c r="D11" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E11" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Blue-Sky-Stream/Gyarados-VMAX-V1?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>Rayquaza</v>
+      </c>
+      <c r="B12" t="str">
+        <v>47/67</v>
+      </c>
+      <c r="C12" t="str">
+        <v>S7R</v>
+      </c>
+      <c r="D12" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E12" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Blue-Sky-Stream/Rayquaza-VMAX-V1-s7R047?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v xml:space="preserve">Leviator </v>
+      </c>
+      <c r="B13" t="str">
+        <v>20/67</v>
+      </c>
+      <c r="C13" t="str">
+        <v>S7R</v>
+      </c>
+      <c r="D13" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E13" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Blue-Sky-Stream/Gyarados-V-V1-s7R020?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>Rayquaza</v>
+      </c>
+      <c r="B14" t="str">
+        <v>46/67</v>
+      </c>
+      <c r="C14" t="str">
+        <v>S7R</v>
+      </c>
+      <c r="D14" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E14" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Blue-Sky-Stream/Rayquaza-V-V1?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>Pyrax</v>
+      </c>
+      <c r="B15" t="str">
+        <v>15/67</v>
+      </c>
+      <c r="C15" t="str">
+        <v>S7R</v>
+      </c>
+      <c r="D15" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E15" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Blue-Sky-Stream/Volcarona-V-V1-s7R015?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>Desseliande</v>
+      </c>
+      <c r="B16" t="str">
+        <v>007/67</v>
+      </c>
+      <c r="C16" t="str">
+        <v>S7R</v>
+      </c>
+      <c r="D16" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E16" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Blue-Sky-Stream/Trevenant-V-V1?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>Dracolosse</v>
+      </c>
+      <c r="B17" t="str">
+        <v>42/67</v>
+      </c>
+      <c r="C17" t="str">
+        <v>S7R</v>
+      </c>
+      <c r="D17" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E17" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Blue-Sky-Stream/Dragonite-V-V1?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>Vmax Duralugon</v>
+      </c>
+      <c r="B18" t="str">
+        <v>285/184</v>
+      </c>
+      <c r="C18" t="str">
+        <v>S8B</v>
+      </c>
+      <c r="D18" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E18" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VMAX-Climax/Duraludon-VMAX-V3-s8b285?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>V Scolocendre</v>
+      </c>
+      <c r="B19" t="str">
+        <v>22/184</v>
+      </c>
+      <c r="C19" t="str">
+        <v>S8B</v>
+      </c>
+      <c r="D19" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E19" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VMAX-Climax/Centiskorch-V-V1-s8b022?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>V Noctali</v>
+      </c>
+      <c r="B20" t="str">
+        <v>100/184</v>
+      </c>
+      <c r="C20" t="str">
+        <v>S8B</v>
+      </c>
+      <c r="D20" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E20" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VMAX-Climax/Umbreon-V-V1-s8b100?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>V Zeraora</v>
+      </c>
+      <c r="B21" t="str">
+        <v>54/184</v>
+      </c>
+      <c r="C21" t="str">
+        <v>S8B</v>
+      </c>
+      <c r="D21" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E21" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VMAX-Climax/Zeraora-V-V1-s8b054?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>V Sulfura</v>
+      </c>
+      <c r="B22" t="str">
+        <v>96/184</v>
+      </c>
+      <c r="C22" t="str">
+        <v>S8B</v>
+      </c>
+      <c r="D22" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E22" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VMAX-Climax/Galarian-Moltres-V-V1-s8b096?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v xml:space="preserve">V Duralugon </v>
+      </c>
+      <c r="B23" t="str">
+        <v>122/184</v>
+      </c>
+      <c r="C23" t="str">
+        <v>S8B</v>
+      </c>
+      <c r="D23" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E23" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VMAX-Climax/Duraludon-V?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>V Mimiqui</v>
+      </c>
+      <c r="B24" t="str">
+        <v>76/184</v>
+      </c>
+      <c r="C24" t="str">
+        <v>S8B</v>
+      </c>
+      <c r="D24" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E24" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VMAX-Climax/Mimikyu-V-V1-s8b076?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>Vmax Rayquaza</v>
+      </c>
+      <c r="B25" t="str">
+        <v>120/184</v>
+      </c>
+      <c r="C25" t="str">
+        <v>S8B</v>
+      </c>
+      <c r="D25" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E25" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VMAX-Climax/Rayquaza-VMAX-V1-s8b120?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>Vmax Pikachu</v>
+      </c>
+      <c r="B26" t="str">
+        <v>46/184</v>
+      </c>
+      <c r="C26" t="str">
+        <v>S8B</v>
+      </c>
+      <c r="D26" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E26" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VMAX-Climax/Pikachu-VMAX-V1-s8b046?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v xml:space="preserve">Vmax Sylveroy </v>
+      </c>
+      <c r="B27" t="str">
+        <v>44/184</v>
+      </c>
+      <c r="C27" t="str">
+        <v>S8B</v>
+      </c>
+      <c r="D27" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E27" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VMAX-Climax/Ice-Rider-Calyrex-VMAX-V1-s8b044?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>Pyroli</v>
+      </c>
+      <c r="B28" t="str">
+        <v>188/184</v>
+      </c>
+      <c r="C28" t="str">
+        <v>S8B</v>
+      </c>
+      <c r="D28" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E28" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VMAX-Climax/Flareon-V2-s8b188?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>Evoli</v>
+      </c>
+      <c r="B29" t="str">
+        <v>210/184</v>
+      </c>
+      <c r="C29" t="str">
+        <v>S8B</v>
+      </c>
+      <c r="D29" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E29" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VMAX-Climax/Eevee-V2-s8b210?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>Hexadron</v>
+      </c>
+      <c r="B30" t="str">
+        <v>201/184</v>
+      </c>
+      <c r="C30" t="str">
+        <v>S8B</v>
+      </c>
+      <c r="D30" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E30" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VMAX-Climax/Falinks-V1-s8b089?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>V Corvaillus</v>
+      </c>
+      <c r="B31" t="str">
+        <v>248/184</v>
+      </c>
+      <c r="C31" t="str">
+        <v>S8B</v>
+      </c>
+      <c r="D31" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E31" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VMAX-Climax/Corviknight-V-V2-s8b248?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>V Mackogneur</v>
+      </c>
+      <c r="B32" t="str">
+        <v>71/172</v>
+      </c>
+      <c r="C32" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D32" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E32" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Machamp-V-s12a071?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>V Amovénus</v>
+      </c>
+      <c r="B33" t="str">
+        <v>68/172</v>
+      </c>
+      <c r="C33" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D33" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E33" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Enamorus-V-s12a068?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>V Cerbyllin</v>
+      </c>
+      <c r="B34" t="str">
+        <v>131/172</v>
+      </c>
+      <c r="C34" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D34" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E34" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Wyrdeer-V-s12a131?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>V Regigigas</v>
+      </c>
+      <c r="B35" t="str">
+        <v>124/172</v>
+      </c>
+      <c r="C35" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D35" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E35" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Regigigas-V-s12a124?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>V Mewtwo</v>
+      </c>
+      <c r="B36" t="str">
+        <v>50/172</v>
+      </c>
+      <c r="C36" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D36" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E36" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Mewtwo-V-s12a050?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>Guérilande</v>
+      </c>
+      <c r="B37" t="str">
+        <v>187/172</v>
+      </c>
+      <c r="C37" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D37" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E37" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Comfey-V2-s12a187?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>Plumeline</v>
+      </c>
+      <c r="B38" t="str">
+        <v>176/172</v>
+      </c>
+      <c r="C38" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D38" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E38" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Oricorio-V2-s12a176?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>Castorno</v>
+      </c>
+      <c r="B39" t="str">
+        <v>200/172</v>
+      </c>
+      <c r="C39" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D39" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E39" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Bibarel-V2-s12a200?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>Energie elect</v>
+      </c>
+      <c r="B40" t="str">
+        <v>254/172</v>
+      </c>
+      <c r="C40" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D40" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E40" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Lightning-Energy-s12a254?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>Vstar Dialga</v>
+      </c>
+      <c r="B41" t="str">
+        <v>101/172</v>
+      </c>
+      <c r="C41" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D41" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E41" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Origin-Forme-Dialga-VSTAR-V1-s12a101?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>Vstar Giratina</v>
+      </c>
+      <c r="B42" t="str">
+        <v>111/172</v>
+      </c>
+      <c r="C42" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D42" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E42" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Giratina-VSTAR-V1-s12a111?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>Vmax Mew</v>
+      </c>
+      <c r="B43" t="str">
+        <v>54/172</v>
+      </c>
+      <c r="C43" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D43" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E43" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Mew-VMAX-s12a054?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>Vstar Regigigas</v>
+      </c>
+      <c r="B44" t="str">
+        <v>125/172</v>
+      </c>
+      <c r="C44" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D44" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E44" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Regigigas-VSTAR-V1-s12a125?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>Vitalité de Flo</v>
+      </c>
+      <c r="B45" t="str">
+        <v>243/172</v>
+      </c>
+      <c r="C45" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D45" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E45" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Gardenias-Vigor-V2-s12a243?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v>V Zacian</v>
+      </c>
+      <c r="B46" t="str">
+        <v>225/172</v>
+      </c>
+      <c r="C46" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D46" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E46" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Zacian-V-V2-s12a225?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>Dracaufeu Radieux</v>
+      </c>
+      <c r="B47" t="str">
+        <v>015/172</v>
+      </c>
+      <c r="C47" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D47" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E47" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Radiant-Charizard-s12a015?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v>Entei V</v>
+      </c>
+      <c r="B48" t="str">
+        <v>213/172</v>
+      </c>
+      <c r="C48" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D48" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E48" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Entei-V-V2-s12a213?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="str">
+        <v>Rayquaza VMAX</v>
+      </c>
+      <c r="B49" t="str">
+        <v>108/172</v>
+      </c>
+      <c r="C49" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D49" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E49" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Rayquaza-VMAX-s12a108?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="str">
+        <v>Palkia Originel VSTAR</v>
+      </c>
+      <c r="B50" t="str">
+        <v>028/172</v>
+      </c>
+      <c r="C50" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D50" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E50" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Origin-Forme-Palkia-VSTAR-V1-s12a028?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="str">
+        <v>Dialga Originel VSTAR</v>
+      </c>
+      <c r="B51" t="str">
+        <v>101/172</v>
+      </c>
+      <c r="C51" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D51" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E51" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Origin-Forme-Dialga-VSTAR-V1-s12a101?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="str">
+        <v>Roublenard</v>
+      </c>
+      <c r="B52" t="str">
+        <v>192/172</v>
+      </c>
+      <c r="C52" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D52" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E52" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Thievul-V2-s12a192?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="str">
+        <v>Salarsen</v>
+      </c>
+      <c r="B53" t="str">
+        <v>181/172</v>
+      </c>
+      <c r="C53" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D53" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E53" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Toxtricity-V2-s12a181?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="str">
+        <v>Ecrémeuf</v>
+      </c>
+      <c r="B54" t="str">
+        <v>199/172</v>
+      </c>
+      <c r="C54" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D54" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E54" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Miltank-V2-s12a199?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="str">
+        <v>Zoroark de Hisui V</v>
+      </c>
+      <c r="B55" t="str">
+        <v>128/172</v>
+      </c>
+      <c r="C55" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D55" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E55" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Hisuian-Zoroark-V-s12a128?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="str">
+        <v>Zeraora V</v>
+      </c>
+      <c r="B56" t="str">
+        <v>040/172</v>
+      </c>
+      <c r="C56" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D56" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E56" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Zeraora-V-s12a040?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="str">
+        <v>Giratina V</v>
+      </c>
+      <c r="B57" t="str">
+        <v>110/172</v>
+      </c>
+      <c r="C57" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D57" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E57" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Giratina-V-s12a110?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="str">
+        <v>Sorcilence</v>
+      </c>
+      <c r="B58" t="str">
+        <v>065/172</v>
+      </c>
+      <c r="C58" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D58" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E58" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Hatterene-V-s12a065?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="str">
+        <v>Carchacrock V</v>
+      </c>
+      <c r="B59" t="str">
+        <v>109/172</v>
+      </c>
+      <c r="C59" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D59" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E59" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Garchomp-V-s12a109?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="str">
+        <v>Recherche Professorale</v>
+      </c>
+      <c r="B60" t="str">
+        <v>248/172</v>
+      </c>
+      <c r="C60" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D60" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E60" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Professors-Research-V2-s12a248?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="str">
+        <v>Energie Psy</v>
+      </c>
+      <c r="B61" t="str">
+        <v>255/172</v>
+      </c>
+      <c r="C61" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D61" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E61" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Psychic-Energy-s12a255?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="str">
+        <v>Brutalibré Radieux</v>
+      </c>
+      <c r="B62" t="str">
+        <v>078/172</v>
+      </c>
+      <c r="C62" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D62" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E62" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Radiant-Hawlucha-s12a078?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="str">
+        <v>Giratina Holo</v>
+      </c>
+      <c r="B63" t="str">
+        <v>10/127</v>
+      </c>
+      <c r="C63" t="str">
+        <v>Platine</v>
+      </c>
+      <c r="D63" t="str">
+        <v>FR</v>
+      </c>
+      <c r="E63" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Platinum/Giratina-Lv63-PL10?language=2&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="str">
+        <v>Giratina VSTAR</v>
+      </c>
+      <c r="B64" t="str">
+        <v>261/172</v>
+      </c>
+      <c r="C64" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D64" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E64" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Giratina-VSTAR-V2-s12a261?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="str">
+        <v>Energie Tênebre</v>
+      </c>
+      <c r="B65" t="str">
+        <v>257/172</v>
+      </c>
+      <c r="C65" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D65" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E65" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Darkness-Energy-s12a257?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="str">
+        <v>Energie Acier</v>
+      </c>
+      <c r="B66" t="str">
+        <v>258/172</v>
+      </c>
+      <c r="C66" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D66" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E66" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Metal-Energy-s12a258?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="str">
+        <v>Energie Feu</v>
+      </c>
+      <c r="B67" t="str">
+        <v>252/172</v>
+      </c>
+      <c r="C67" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D67" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E67" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Fire-Energy-s12a252?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="str">
+        <v>Regigigas VSTAR</v>
+      </c>
+      <c r="B68" t="str">
+        <v>233/172</v>
+      </c>
+      <c r="C68" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D68" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E68" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Regigigas-VSTAR-V2-s12a233?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="str">
+        <v>Entei V</v>
+      </c>
+      <c r="B69" t="str">
+        <v>213/172</v>
+      </c>
+      <c r="C69" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D69" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E69" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Entei-V-V2-s12a213?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="str">
+        <v xml:space="preserve">Suicune </v>
+      </c>
+      <c r="B70" t="str">
+        <v>215/172</v>
+      </c>
+      <c r="C70" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D70" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E70" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Suicune-V-V2-s12a215?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="str">
+        <v>Clamiral</v>
+      </c>
+      <c r="B71" t="str">
+        <v>229/172</v>
+      </c>
+      <c r="C71" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D71" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E71" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Hisuian-Samurott-V-V2-s12a229?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="str">
+        <v>Darkrai VSTAR</v>
+      </c>
+      <c r="B72" t="str">
+        <v>228/172</v>
+      </c>
+      <c r="C72" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D72" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E72" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Darkrai-VSTAR-s12a228?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="str">
+        <v>Deoxy Vmax</v>
+      </c>
+      <c r="B73" t="str">
+        <v>222/172</v>
+      </c>
+      <c r="C73" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D73" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E73" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Deoxys-VMAX-s12a222?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="str">
+        <v>Zacian V</v>
+      </c>
+      <c r="B74" t="str">
+        <v>225/172</v>
+      </c>
+      <c r="C74" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D74" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E74" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Zacian-V-V2-s12a225?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="str">
+        <v>Hoopa</v>
+      </c>
+      <c r="B75" t="str">
+        <v>231/172</v>
+      </c>
+      <c r="C75" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D75" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E75" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Hoopa-V-s12a231?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="str">
+        <v>Clamiral Vstar</v>
+      </c>
+      <c r="B76" t="str">
+        <v>230/172</v>
+      </c>
+      <c r="C76" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D76" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E76" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Hisuian-Samurott-VSTAR-V2-s12a230?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="str">
+        <v>Raikou</v>
+      </c>
+      <c r="B77" t="str">
+        <v>218/172</v>
+      </c>
+      <c r="C77" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D77" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E77" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Raikou-V-V2-s12a218?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="str">
+        <v>Drascore</v>
+      </c>
+      <c r="B78" t="str">
+        <v>227/172</v>
+      </c>
+      <c r="C78" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D78" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E78" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Drapion-V-V2-s12a227?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="str">
+        <v>Keldeo</v>
+      </c>
+      <c r="B79" t="str">
+        <v>179/172</v>
+      </c>
+      <c r="C79" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D79" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E79" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Keldeo-V2-s12a179?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="str">
+        <v>Insolourdo</v>
+      </c>
+      <c r="B80" t="str">
+        <v>198/172</v>
+      </c>
+      <c r="C80" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D80" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E80" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Dunsparce-V2-s12a198?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="str">
+        <v>Maganon</v>
+      </c>
+      <c r="B81" t="str">
+        <v>175/172</v>
+      </c>
+      <c r="C81" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D81" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E81" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Magmortar-V2-s12a175?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="str">
+        <v>Locklass</v>
+      </c>
+      <c r="B82" t="str">
+        <v>177/172</v>
+      </c>
+      <c r="C82" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D82" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E82" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Lapras-V2-s12a177?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="str">
+        <v>Elekable</v>
+      </c>
+      <c r="B83" t="str">
+        <v>180/172</v>
+      </c>
+      <c r="C83" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D83" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E83" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Electivire-V2-s12a180?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="str">
+        <v>Séléroc</v>
+      </c>
+      <c r="B84" t="str">
+        <v>184/172</v>
+      </c>
+      <c r="C84" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D84" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E84" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Lunatone-V2-s12a184?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="str">
+        <v>Electhor de Galar</v>
+      </c>
+      <c r="B85" t="str">
+        <v>188/172</v>
+      </c>
+      <c r="C85" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D85" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E85" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Galarian-Zapdos-V2-s12a188?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="str">
+        <v>Absol</v>
+      </c>
+      <c r="B86" t="str">
+        <v>191/172</v>
+      </c>
+      <c r="C86" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D86" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E86" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Absol-V2-s12a191?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="str">
+        <v>Roublenard</v>
+      </c>
+      <c r="B87" t="str">
+        <v>192/172</v>
+      </c>
+      <c r="C87" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D87" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E87" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Thievul-V2-s12a192?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="str">
+        <v>Magnézone</v>
+      </c>
+      <c r="B88" t="str">
+        <v>193/172</v>
+      </c>
+      <c r="C88" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D88" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E88" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Magnezone-V2-s12a193?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="str">
+        <v>Voltorbe de Hisui</v>
+      </c>
+      <c r="B89" t="str">
+        <v>173/172</v>
+      </c>
+      <c r="C89" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D89" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E89" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Hisuian-Voltorb-V2-s12a173?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="str">
+        <v>Altaria</v>
+      </c>
+      <c r="B90" t="str">
+        <v>194/172</v>
+      </c>
+      <c r="C90" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D90" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E90" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Altaria-V2-s12a194?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="str">
+        <v>Mew</v>
+      </c>
+      <c r="B91" t="str">
+        <v>183/172</v>
+      </c>
+      <c r="C91" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D91" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E91" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Mew-V2-s12a183?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="str">
+        <v>Melokrik</v>
+      </c>
+      <c r="B92" t="str">
+        <v>174/172</v>
+      </c>
+      <c r="C92" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D92" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E92" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Kricketune-V2-s12a174?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="str">
+        <v>Diancy</v>
+      </c>
+      <c r="B93" t="str">
+        <v>186/172</v>
+      </c>
+      <c r="C93" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D93" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E93" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Diancie-V2-s12a186?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="str">
+        <v>Sulfura Galar</v>
+      </c>
+      <c r="B94" t="str">
+        <v>190/172</v>
+      </c>
+      <c r="C94" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D94" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E94" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Galarian-Moltres-V2-s12a190?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="str">
+        <v>Muplodocus</v>
+      </c>
+      <c r="B95" t="str">
+        <v>196/172</v>
+      </c>
+      <c r="C95" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D95" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E95" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Hisuian-Goodra-V2-s12a196?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="str">
+        <v>Artikodin Galar</v>
+      </c>
+      <c r="B96" t="str">
+        <v>182/172</v>
+      </c>
+      <c r="C96" t="str">
+        <v>S12A</v>
+      </c>
+      <c r="D96" t="str">
+        <v>JP</v>
+      </c>
+      <c r="E96" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Galarian-Articuno-V2-s12a182?language=7&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="str">
+        <v>Tortank Ex</v>
+      </c>
+      <c r="B97" t="str">
+        <v>200/165</v>
+      </c>
+      <c r="C97">
+        <v>151</v>
+      </c>
+      <c r="D97" t="str">
+        <v>FR</v>
+      </c>
+      <c r="E97" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/151/Blastoise-ex-V3-MEW200?language=2&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="str">
+        <v>Charisme de Giovanni</v>
+      </c>
+      <c r="B98" t="str">
+        <v>204/165</v>
+      </c>
+      <c r="C98">
+        <v>151</v>
+      </c>
+      <c r="D98" t="str">
+        <v>FR</v>
+      </c>
+      <c r="E98" t="str">
+        <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/151/Giovannis-Charisma-V3-MEW204?language=2&amp;minCondition=2&amp;isSigned=N&amp;isPlayset=N&amp;isAltered=N</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:F98"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>